<commit_message>
Tidplan version 1 should be finished
</commit_message>
<xml_diff>
--- a/doc/projektplan/05Tidplan01.xlsx
+++ b/doc/projektplan/05Tidplan01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.liu.se\home\emiha868\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.liu.se\home\emiha868\Desktop\tsea29-taxi\doc\projektplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -829,6 +829,105 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
@@ -841,57 +940,49 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -903,97 +994,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1333,29 +1333,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
+      <c r="A1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
       <c r="AMA1"/>
       <c r="AMB1"/>
       <c r="AMC1"/>
@@ -1368,40 +1368,40 @@
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="89"/>
+      <c r="B2" s="51"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="52"/>
     </row>
     <row r="3" spans="1:1024" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="88"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="87">
+      <c r="D3" s="55">
         <v>2</v>
       </c>
-      <c r="E3" s="87"/>
+      <c r="E3" s="55"/>
       <c r="F3" s="56"/>
       <c r="G3" s="57" t="s">
         <v>3</v>
@@ -1424,89 +1424,89 @@
       <c r="U3" s="58"/>
     </row>
     <row r="4" spans="1:1024" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="49"/>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="60"/>
     </row>
     <row r="5" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="86"/>
+      <c r="B5" s="62"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="50" t="s">
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="49"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
     </row>
     <row r="6" spans="1:1024" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="84"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="67"/>
       <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="46"/>
-      <c r="R6" s="46"/>
-      <c r="S6" s="46"/>
-      <c r="T6" s="46"/>
-      <c r="U6" s="46"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="68"/>
+      <c r="S6" s="68"/>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
       <c r="V6"/>
       <c r="W6"/>
       <c r="AMA6"/>
@@ -1524,12 +1524,12 @@
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="81"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="48"/>
       <c r="F7" s="7" t="s">
         <v>15</v>
       </c>
@@ -1581,12 +1581,12 @@
       <c r="A8" s="8">
         <v>1</v>
       </c>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="79"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="10">
         <v>1120</v>
       </c>
@@ -1633,12 +1633,12 @@
       <c r="A9" s="8">
         <v>2</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="79"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="10">
         <v>420</v>
       </c>
@@ -1667,12 +1667,12 @@
       <c r="A10" s="8">
         <v>3</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="79"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="10">
         <v>700</v>
       </c>
@@ -1698,46 +1698,46 @@
       </c>
     </row>
     <row r="11" spans="1:1024" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="83"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="84"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="67"/>
       <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
-      <c r="R11" s="46"/>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="68"/>
+      <c r="Q11" s="68"/>
+      <c r="R11" s="68"/>
+      <c r="S11" s="68"/>
+      <c r="T11" s="68"/>
+      <c r="U11" s="68"/>
     </row>
     <row r="12" spans="1:1024" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="81"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="7" t="s">
         <v>15</v>
       </c>
@@ -1789,12 +1789,12 @@
       <c r="A13" s="8">
         <v>4</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="79"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="10">
         <v>80</v>
       </c>
@@ -1829,12 +1829,12 @@
       <c r="A14" s="8">
         <v>5</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="79"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="10">
         <v>45</v>
       </c>
@@ -1869,12 +1869,12 @@
       <c r="A15" s="8">
         <v>6</v>
       </c>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="79"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="10">
         <v>45</v>
       </c>
@@ -1909,12 +1909,12 @@
       <c r="A16" s="8">
         <v>7</v>
       </c>
-      <c r="B16" s="77" t="s">
+      <c r="B16" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="79"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="10">
         <v>45</v>
       </c>
@@ -1949,12 +1949,12 @@
       <c r="A17" s="8">
         <v>8</v>
       </c>
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="78"/>
-      <c r="D17" s="78"/>
-      <c r="E17" s="79"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="10">
         <v>75</v>
       </c>
@@ -1989,12 +1989,12 @@
       <c r="A18" s="8">
         <v>9</v>
       </c>
-      <c r="B18" s="77" t="s">
+      <c r="B18" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="79"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="10">
         <v>65</v>
       </c>
@@ -2029,12 +2029,12 @@
       <c r="A19" s="8">
         <v>10</v>
       </c>
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="79"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="10">
         <v>3</v>
       </c>
@@ -2065,12 +2065,12 @@
       <c r="A20" s="8">
         <v>11</v>
       </c>
-      <c r="B20" s="77" t="s">
+      <c r="B20" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="79"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="10">
         <v>20</v>
       </c>
@@ -2103,12 +2103,12 @@
       <c r="A21" s="8">
         <v>12</v>
       </c>
-      <c r="B21" s="77" t="s">
+      <c r="B21" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="78"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="79"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="42"/>
       <c r="F21" s="10">
         <v>21</v>
       </c>
@@ -2143,12 +2143,12 @@
       <c r="A22" s="8">
         <v>13</v>
       </c>
-      <c r="B22" s="77" t="s">
+      <c r="B22" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="79"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="10">
         <f>(420-SUM(F13:F21))</f>
         <v>21</v>
@@ -2187,12 +2187,12 @@
       <c r="A23" s="8">
         <v>14</v>
       </c>
-      <c r="B23" s="77" t="s">
+      <c r="B23" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="79"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="10">
         <f>SUM(F13:F22)</f>
         <v>420</v>
@@ -2237,46 +2237,46 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="82" t="s">
+      <c r="A24" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="84"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="67"/>
       <c r="F24" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="47" t="s">
+      <c r="H24" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
-      <c r="P24" s="47"/>
-      <c r="Q24" s="47"/>
-      <c r="R24" s="47"/>
-      <c r="S24" s="47"/>
-      <c r="T24" s="47"/>
-      <c r="U24" s="47"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="69"/>
+      <c r="Q24" s="69"/>
+      <c r="R24" s="69"/>
+      <c r="S24" s="69"/>
+      <c r="T24" s="69"/>
+      <c r="U24" s="69"/>
     </row>
     <row r="25" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="81"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="48"/>
       <c r="F25" s="7" t="s">
         <v>15</v>
       </c>
@@ -2328,12 +2328,12 @@
       <c r="A26" s="8">
         <v>15</v>
       </c>
-      <c r="B26" s="77" t="s">
+      <c r="B26" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="79"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="10">
         <v>50</v>
       </c>
@@ -2372,12 +2372,12 @@
       <c r="A27" s="8">
         <v>16</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="79"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="42"/>
       <c r="F27" s="10">
         <v>60</v>
       </c>
@@ -2414,12 +2414,12 @@
       <c r="A28" s="8">
         <v>17</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="45"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="72"/>
       <c r="F28" s="16">
         <v>8</v>
       </c>
@@ -2456,12 +2456,12 @@
       <c r="A29" s="8">
         <v>18</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="72"/>
       <c r="F29" s="16">
         <v>5</v>
       </c>
@@ -2496,12 +2496,12 @@
       <c r="A30" s="8">
         <v>19</v>
       </c>
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="45"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="72"/>
       <c r="F30" s="16">
         <v>15</v>
       </c>
@@ -2536,12 +2536,12 @@
       <c r="A31" s="8">
         <v>20</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="45"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="72"/>
       <c r="F31" s="16">
         <v>15</v>
       </c>
@@ -2576,12 +2576,12 @@
       <c r="A32" s="8">
         <v>21</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="45"/>
+      <c r="C32" s="71"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="72"/>
       <c r="F32" s="16">
         <v>15</v>
       </c>
@@ -2618,12 +2618,12 @@
       <c r="A33" s="8">
         <v>22</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="45"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="72"/>
       <c r="F33" s="16">
         <v>15</v>
       </c>
@@ -2658,12 +2658,12 @@
       <c r="A34" s="8">
         <v>23</v>
       </c>
-      <c r="B34" s="43" t="s">
+      <c r="B34" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="45"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="72"/>
       <c r="F34" s="16">
         <v>10</v>
       </c>
@@ -2700,12 +2700,12 @@
       <c r="A35" s="8">
         <v>24</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="45"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="72"/>
       <c r="F35" s="16">
         <v>10</v>
       </c>
@@ -2740,12 +2740,12 @@
       <c r="A36" s="8">
         <v>25</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="45"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="72"/>
       <c r="F36" s="16">
         <v>10</v>
       </c>
@@ -2780,12 +2780,12 @@
       <c r="A37" s="8">
         <v>26</v>
       </c>
-      <c r="B37" s="43" t="s">
+      <c r="B37" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="45"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="72"/>
       <c r="F37" s="16">
         <v>8</v>
       </c>
@@ -2822,12 +2822,12 @@
       <c r="A38" s="8">
         <v>27</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="45"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="72"/>
       <c r="F38" s="16">
         <v>10</v>
       </c>
@@ -2862,12 +2862,12 @@
       <c r="A39" s="8">
         <v>29</v>
       </c>
-      <c r="B39" s="43" t="s">
+      <c r="B39" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="45"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="72"/>
       <c r="F39" s="16">
         <v>20</v>
       </c>
@@ -2902,12 +2902,12 @@
       <c r="A40" s="8">
         <v>30</v>
       </c>
-      <c r="B40" s="43" t="s">
+      <c r="B40" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="45"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="72"/>
       <c r="F40" s="16">
         <v>10</v>
       </c>
@@ -2942,12 +2942,12 @@
       <c r="A41" s="8">
         <v>31</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="B41" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="44"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="45"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="72"/>
       <c r="F41" s="16">
         <v>8</v>
       </c>
@@ -2982,12 +2982,12 @@
       <c r="A42" s="8">
         <v>32</v>
       </c>
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="45"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="72"/>
       <c r="F42" s="16">
         <v>5</v>
       </c>
@@ -3022,12 +3022,12 @@
       <c r="A43" s="8">
         <v>33</v>
       </c>
-      <c r="B43" s="43" t="s">
+      <c r="B43" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="45"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="72"/>
       <c r="F43" s="16">
         <v>5</v>
       </c>
@@ -3062,12 +3062,12 @@
       <c r="A44" s="8">
         <v>34</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="45"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="72"/>
       <c r="F44" s="16">
         <v>5</v>
       </c>
@@ -3102,12 +3102,12 @@
       <c r="A45" s="8">
         <v>35</v>
       </c>
-      <c r="B45" s="43" t="s">
+      <c r="B45" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="45"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="72"/>
       <c r="F45" s="16">
         <v>5</v>
       </c>
@@ -3142,12 +3142,12 @@
       <c r="A46" s="8">
         <v>36</v>
       </c>
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="45"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71"/>
+      <c r="E46" s="72"/>
       <c r="F46" s="16">
         <v>10</v>
       </c>
@@ -3184,12 +3184,12 @@
       <c r="A47" s="8">
         <v>37</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="45"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="72"/>
       <c r="F47" s="16">
         <v>5</v>
       </c>
@@ -3224,12 +3224,12 @@
       <c r="A48" s="8">
         <v>38</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="44"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="45"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="72"/>
       <c r="F48" s="16">
         <v>10</v>
       </c>
@@ -3266,12 +3266,12 @@
       <c r="A49" s="8">
         <v>39</v>
       </c>
-      <c r="B49" s="43" t="s">
+      <c r="B49" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="45"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="72"/>
       <c r="F49" s="16">
         <v>8</v>
       </c>
@@ -3308,12 +3308,12 @@
       <c r="A50" s="8">
         <v>40</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="B50" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="45"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="72"/>
       <c r="F50" s="16">
         <v>10</v>
       </c>
@@ -3350,12 +3350,12 @@
       <c r="A51" s="8">
         <v>41</v>
       </c>
-      <c r="B51" s="43" t="s">
+      <c r="B51" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44"/>
-      <c r="E51" s="45"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="71"/>
+      <c r="E51" s="72"/>
       <c r="F51" s="16">
         <v>5</v>
       </c>
@@ -3390,12 +3390,12 @@
       <c r="A52" s="8">
         <v>42</v>
       </c>
-      <c r="B52" s="43" t="s">
+      <c r="B52" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="45"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="71"/>
+      <c r="E52" s="72"/>
       <c r="F52" s="16">
         <v>5</v>
       </c>
@@ -3430,12 +3430,12 @@
       <c r="A53" s="8">
         <v>43</v>
       </c>
-      <c r="B53" s="43" t="s">
+      <c r="B53" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="44"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="45"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="71"/>
+      <c r="E53" s="72"/>
       <c r="F53" s="16">
         <v>10</v>
       </c>
@@ -3470,12 +3470,12 @@
       <c r="A54" s="8">
         <v>44</v>
       </c>
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="44"/>
-      <c r="D54" s="44"/>
-      <c r="E54" s="45"/>
+      <c r="C54" s="71"/>
+      <c r="D54" s="71"/>
+      <c r="E54" s="72"/>
       <c r="F54" s="16">
         <v>10</v>
       </c>
@@ -3510,12 +3510,12 @@
       <c r="A55" s="8">
         <v>45</v>
       </c>
-      <c r="B55" s="43" t="s">
+      <c r="B55" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="C55" s="44"/>
-      <c r="D55" s="44"/>
-      <c r="E55" s="45"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="71"/>
+      <c r="E55" s="72"/>
       <c r="F55" s="16">
         <v>10</v>
       </c>
@@ -3552,12 +3552,12 @@
       <c r="A56" s="8">
         <v>46</v>
       </c>
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="44"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="45"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="71"/>
+      <c r="E56" s="72"/>
       <c r="F56" s="16">
         <v>15</v>
       </c>
@@ -3594,12 +3594,12 @@
       <c r="A57" s="8">
         <v>47</v>
       </c>
-      <c r="B57" s="40" t="s">
+      <c r="B57" s="73" t="s">
         <v>63</v>
       </c>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="42"/>
+      <c r="C57" s="74"/>
+      <c r="D57" s="74"/>
+      <c r="E57" s="75"/>
       <c r="F57" s="16">
         <v>15</v>
       </c>
@@ -3636,12 +3636,12 @@
       <c r="A58" s="8">
         <v>48</v>
       </c>
-      <c r="B58" s="43" t="s">
+      <c r="B58" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="C58" s="44"/>
-      <c r="D58" s="44"/>
-      <c r="E58" s="45"/>
+      <c r="C58" s="71"/>
+      <c r="D58" s="71"/>
+      <c r="E58" s="72"/>
       <c r="F58" s="16">
         <v>40</v>
       </c>
@@ -3682,12 +3682,12 @@
       <c r="A59" s="8">
         <v>49</v>
       </c>
-      <c r="B59" s="43" t="s">
+      <c r="B59" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="44"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="45"/>
+      <c r="C59" s="71"/>
+      <c r="D59" s="71"/>
+      <c r="E59" s="72"/>
       <c r="F59" s="16">
         <v>30</v>
       </c>
@@ -3726,12 +3726,12 @@
       <c r="A60" s="8">
         <v>50</v>
       </c>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="C60" s="44"/>
-      <c r="D60" s="44"/>
-      <c r="E60" s="45"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="71"/>
+      <c r="E60" s="72"/>
       <c r="F60" s="16">
         <v>30</v>
       </c>
@@ -3770,12 +3770,12 @@
       <c r="A61" s="8">
         <v>51</v>
       </c>
-      <c r="B61" s="43" t="s">
+      <c r="B61" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="45"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="71"/>
+      <c r="E61" s="72"/>
       <c r="F61" s="16">
         <v>50</v>
       </c>
@@ -3814,12 +3814,12 @@
       <c r="A62" s="8">
         <v>52</v>
       </c>
-      <c r="B62" s="43" t="s">
+      <c r="B62" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="C62" s="44"/>
-      <c r="D62" s="44"/>
-      <c r="E62" s="45"/>
+      <c r="C62" s="71"/>
+      <c r="D62" s="71"/>
+      <c r="E62" s="72"/>
       <c r="F62" s="16">
         <v>20</v>
       </c>
@@ -3856,12 +3856,12 @@
       <c r="A63" s="8">
         <v>53</v>
       </c>
-      <c r="B63" s="43" t="s">
+      <c r="B63" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="45"/>
+      <c r="C63" s="71"/>
+      <c r="D63" s="71"/>
+      <c r="E63" s="72"/>
       <c r="F63" s="16">
         <v>20</v>
       </c>
@@ -3898,12 +3898,12 @@
       <c r="A64" s="8">
         <v>54</v>
       </c>
-      <c r="B64" s="43" t="s">
+      <c r="B64" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="C64" s="44"/>
-      <c r="D64" s="44"/>
-      <c r="E64" s="45"/>
+      <c r="C64" s="71"/>
+      <c r="D64" s="71"/>
+      <c r="E64" s="72"/>
       <c r="F64" s="16">
         <v>5</v>
       </c>
@@ -3946,12 +3946,12 @@
       <c r="A65" s="8">
         <v>55</v>
       </c>
-      <c r="B65" s="43" t="s">
+      <c r="B65" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="C65" s="44"/>
-      <c r="D65" s="44"/>
-      <c r="E65" s="45"/>
+      <c r="C65" s="71"/>
+      <c r="D65" s="71"/>
+      <c r="E65" s="72"/>
       <c r="F65" s="16">
         <v>15</v>
       </c>
@@ -3994,12 +3994,12 @@
       <c r="A66" s="8">
         <v>56</v>
       </c>
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C66" s="44"/>
-      <c r="D66" s="44"/>
-      <c r="E66" s="45"/>
+      <c r="C66" s="71"/>
+      <c r="D66" s="71"/>
+      <c r="E66" s="72"/>
       <c r="F66" s="16">
         <v>21</v>
       </c>
@@ -4038,12 +4038,12 @@
       <c r="A67" s="8">
         <v>57</v>
       </c>
-      <c r="B67" s="43" t="s">
+      <c r="B67" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="44"/>
-      <c r="D67" s="44"/>
-      <c r="E67" s="45"/>
+      <c r="C67" s="71"/>
+      <c r="D67" s="71"/>
+      <c r="E67" s="72"/>
       <c r="F67" s="16">
         <v>12</v>
       </c>
@@ -4080,12 +4080,12 @@
       <c r="A68" s="8">
         <v>58</v>
       </c>
-      <c r="B68" s="43" t="s">
+      <c r="B68" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="44"/>
-      <c r="D68" s="44"/>
-      <c r="E68" s="45"/>
+      <c r="C68" s="71"/>
+      <c r="D68" s="71"/>
+      <c r="E68" s="72"/>
       <c r="F68" s="16">
         <f>(700-SUM(F26:F67))</f>
         <v>55</v>
@@ -4134,12 +4134,12 @@
       <c r="A69" s="8">
         <v>59</v>
       </c>
-      <c r="B69" s="43" t="s">
+      <c r="B69" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="44"/>
-      <c r="D69" s="44"/>
-      <c r="E69" s="45"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="71"/>
+      <c r="E69" s="72"/>
       <c r="F69" s="16">
         <f>SUM(F26:F68)</f>
         <v>700</v>
@@ -4180,79 +4180,144 @@
     </row>
     <row r="70" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
-      <c r="B70" s="90" t="s">
+      <c r="B70" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C70" s="91"/>
-      <c r="D70" s="91"/>
-      <c r="E70" s="92"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="45"/>
       <c r="F70" s="17">
         <f>SUM(F23,F69)</f>
         <v>1120</v>
       </c>
       <c r="G70" s="17">
-        <f>SUM(G13:G22,G26:G68)</f>
+        <f t="shared" ref="G70:U70" si="6">SUM(G13:G22,G26:G68)</f>
         <v>0</v>
       </c>
       <c r="H70" s="17">
-        <f>SUM(H13:H22,H26:H68)</f>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="I70" s="17">
-        <f>SUM(I13:I22,I26:I68)</f>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="J70" s="17">
-        <f>SUM(J13:J22,J26:J68)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="K70" s="17">
-        <f>SUM(K13:K22,K26:K68)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L70" s="17">
-        <f>SUM(L13:L22,L26:L68)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M70" s="17">
-        <f>SUM(M13:M22,M26:M68)</f>
+        <f t="shared" si="6"/>
         <v>133</v>
       </c>
       <c r="N70" s="17">
-        <f>SUM(N13:N22,N26:N68)</f>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="O70" s="17">
-        <f>SUM(O13:O22,O26:O68)</f>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="P70" s="17">
-        <f>SUM(P13:P22,P26:P68)</f>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="Q70" s="17">
-        <f>SUM(Q13:Q22,Q26:Q68)</f>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="R70" s="17">
-        <f>SUM(R13:R22,R26:R68)</f>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="S70" s="17">
-        <f>SUM(S13:S22,S26:S68)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T70" s="17">
-        <f>SUM(T13:T22,T26:T68)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U70" s="17">
-        <f>SUM(U13:U22,U26:U68)</f>
+        <f t="shared" si="6"/>
         <v>1120</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="81">
+    <mergeCell ref="B66:E66"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="B38:E38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="H24:U24"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="H11:U11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="H6:U6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="G4:O4"/>
+    <mergeCell ref="P4:U5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="G5:O5"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:U2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="P3:U3"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B20:E20"/>
@@ -4262,40 +4327,6 @@
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="B23:E23"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:U2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:O3"/>
-    <mergeCell ref="P3:U3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="G4:O4"/>
-    <mergeCell ref="P4:U5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:O5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="H6:U6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="H11:U11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="H24:U24"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="A24:E24"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B34:E34"/>
     <mergeCell ref="B46:E46"/>
@@ -4303,37 +4334,6 @@
     <mergeCell ref="B36:E36"/>
     <mergeCell ref="B37:E37"/>
     <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="B69:E69"/>
   </mergeCells>
   <conditionalFormatting sqref="V26:V68">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
@@ -4372,236 +4372,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="52"/>
-      <c r="AD1" s="52"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
     </row>
     <row r="2" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="72"/>
+      <c r="B2" s="76"/>
       <c r="C2" s="18"/>
-      <c r="D2" s="73">
+      <c r="D2" s="77">
         <f>Basplan!D2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="73"/>
-      <c r="X2" s="73"/>
-      <c r="Y2" s="73"/>
-      <c r="Z2" s="73"/>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="73"/>
-      <c r="AD2" s="73"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
+      <c r="X2" s="77"/>
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="77"/>
+      <c r="AA2" s="77"/>
+      <c r="AB2" s="77"/>
+      <c r="AC2" s="77"/>
+      <c r="AD2" s="77"/>
     </row>
     <row r="3" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="74"/>
+      <c r="B3" s="78"/>
       <c r="C3" s="19"/>
-      <c r="D3" s="75">
+      <c r="D3" s="79">
         <f>Basplan!D3</f>
         <v>2</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="55" t="s">
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="76"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="76"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="76"/>
-      <c r="AA3" s="76"/>
-      <c r="AB3" s="76"/>
-      <c r="AC3" s="76"/>
-      <c r="AD3" s="76"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="80"/>
+      <c r="AA3" s="80"/>
+      <c r="AB3" s="80"/>
+      <c r="AC3" s="80"/>
+      <c r="AD3" s="80"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="66"/>
+      <c r="B4" s="81"/>
       <c r="C4" s="20"/>
-      <c r="D4" s="67">
+      <c r="D4" s="82">
         <f>Basplan!D4</f>
         <v>0</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="66" t="s">
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="68"/>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="68"/>
-      <c r="S4" s="68"/>
-      <c r="T4" s="68"/>
-      <c r="U4" s="68"/>
-      <c r="V4" s="68"/>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="68"/>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="68"/>
-      <c r="AB4" s="68"/>
-      <c r="AC4" s="68"/>
-      <c r="AD4" s="68"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="83"/>
+      <c r="U4" s="83"/>
+      <c r="V4" s="83"/>
+      <c r="W4" s="83"/>
+      <c r="X4" s="83"/>
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="83"/>
+      <c r="AA4" s="83"/>
+      <c r="AB4" s="83"/>
+      <c r="AC4" s="83"/>
+      <c r="AD4" s="83"/>
     </row>
     <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="69"/>
+      <c r="B5" s="84"/>
       <c r="C5" s="21"/>
-      <c r="D5" s="70">
+      <c r="D5" s="85">
         <f>Basplan!D5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="71"/>
-      <c r="S5" s="71"/>
-      <c r="T5" s="71"/>
-      <c r="U5" s="71"/>
-      <c r="V5" s="71"/>
-      <c r="W5" s="71"/>
-      <c r="X5" s="71"/>
-      <c r="Y5" s="71"/>
-      <c r="Z5" s="71"/>
-      <c r="AA5" s="71"/>
-      <c r="AB5" s="71"/>
-      <c r="AC5" s="71"/>
-      <c r="AD5" s="71"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
+      <c r="V5" s="86"/>
+      <c r="W5" s="86"/>
+      <c r="X5" s="86"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="86"/>
+      <c r="AA5" s="86"/>
+      <c r="AB5" s="86"/>
+      <c r="AC5" s="86"/>
+      <c r="AD5" s="86"/>
     </row>
     <row r="6" spans="1:30" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="63" t="s">
+      <c r="B6" s="87"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="63"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="63"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="63"/>
-      <c r="U6" s="63"/>
-      <c r="V6" s="63"/>
-      <c r="W6" s="63"/>
-      <c r="X6" s="63"/>
-      <c r="Y6" s="63"/>
-      <c r="Z6" s="63"/>
-      <c r="AA6" s="63"/>
-      <c r="AB6" s="63"/>
-      <c r="AC6" s="63"/>
-      <c r="AD6" s="63"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="88"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="88"/>
+      <c r="P6" s="88"/>
+      <c r="Q6" s="88"/>
+      <c r="R6" s="88"/>
+      <c r="S6" s="88"/>
+      <c r="T6" s="88"/>
+      <c r="U6" s="88"/>
+      <c r="V6" s="88"/>
+      <c r="W6" s="88"/>
+      <c r="X6" s="88"/>
+      <c r="Y6" s="88"/>
+      <c r="Z6" s="88"/>
+      <c r="AA6" s="88"/>
+      <c r="AB6" s="88"/>
+      <c r="AC6" s="88"/>
+      <c r="AD6" s="88"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
       <c r="G7" s="7">
         <f>Basplan!H7</f>
         <v>40</v>
@@ -4700,11 +4700,11 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" s="25"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
       <c r="G8" s="26"/>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
@@ -4735,11 +4735,11 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" s="25"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="90"/>
       <c r="G9" s="30"/>
       <c r="H9" s="31"/>
       <c r="I9" s="31"/>
@@ -4770,11 +4770,11 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" s="25"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
       <c r="G10" s="30"/>
       <c r="H10" s="31"/>
       <c r="I10" s="31"/>
@@ -4805,11 +4805,11 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" s="25"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
       <c r="G11" s="30"/>
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
@@ -4840,11 +4840,11 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" s="25"/>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
       <c r="G12" s="30"/>
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
@@ -4875,11 +4875,11 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" s="25"/>
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
       <c r="G13" s="30"/>
       <c r="H13" s="31"/>
       <c r="I13" s="31"/>
@@ -4910,11 +4910,11 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" s="25"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
       <c r="G14" s="30"/>
       <c r="H14" s="31"/>
       <c r="I14" s="31"/>
@@ -4945,11 +4945,11 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" s="25"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
       <c r="G15" s="30"/>
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
@@ -4980,11 +4980,11 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" s="25"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
       <c r="G16" s="30"/>
       <c r="H16" s="31"/>
       <c r="I16" s="31"/>
@@ -5015,11 +5015,11 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="25"/>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
       <c r="G17" s="30"/>
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
@@ -5050,11 +5050,11 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="25"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="90"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
       <c r="G18" s="30"/>
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
@@ -5085,11 +5085,11 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="25"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="90"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="90"/>
       <c r="G19" s="30"/>
       <c r="H19" s="31"/>
       <c r="I19" s="31"/>
@@ -5120,11 +5120,11 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="25"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
       <c r="G20" s="30"/>
       <c r="H20" s="31"/>
       <c r="I20" s="31"/>
@@ -5155,11 +5155,11 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="25"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
       <c r="G21" s="30"/>
       <c r="H21" s="31"/>
       <c r="I21" s="31"/>
@@ -5190,11 +5190,11 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="25"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
       <c r="G22" s="30"/>
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
@@ -5225,11 +5225,11 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="25"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
       <c r="G23" s="30"/>
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
@@ -5260,11 +5260,11 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="25"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="90"/>
+      <c r="F24" s="90"/>
       <c r="G24" s="30"/>
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
@@ -5295,11 +5295,11 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="25"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90"/>
+      <c r="F25" s="90"/>
       <c r="G25" s="30"/>
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
@@ -5330,11 +5330,11 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="25"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
       <c r="G26" s="30"/>
       <c r="H26" s="31"/>
       <c r="I26" s="31"/>
@@ -5365,11 +5365,11 @@
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="25"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="90"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
       <c r="G27" s="30"/>
       <c r="H27" s="31"/>
       <c r="I27" s="31"/>
@@ -5400,11 +5400,11 @@
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28" s="34"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
       <c r="G28" s="30"/>
       <c r="H28" s="31"/>
       <c r="I28" s="31"/>
@@ -5435,11 +5435,11 @@
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29" s="34"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="90"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="90"/>
       <c r="G29" s="30"/>
       <c r="H29" s="31"/>
       <c r="I29" s="31"/>
@@ -5470,11 +5470,11 @@
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30" s="25"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
       <c r="G30" s="30"/>
       <c r="H30" s="31"/>
       <c r="I30" s="31"/>
@@ -5505,11 +5505,11 @@
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="25"/>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="90"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
       <c r="G31" s="30"/>
       <c r="H31" s="31"/>
       <c r="I31" s="31"/>
@@ -5540,11 +5540,11 @@
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="25"/>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
       <c r="G32" s="30"/>
       <c r="H32" s="31"/>
       <c r="I32" s="31"/>
@@ -5575,11 +5575,11 @@
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="25"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
       <c r="G33" s="35"/>
       <c r="H33" s="36"/>
       <c r="I33" s="36"/>
@@ -5610,13 +5610,13 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="92"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="92"/>
       <c r="G34" s="38">
         <f t="shared" ref="G34:AD34" si="1">SUM(G8:G33)</f>
         <v>0</v>
@@ -5716,6 +5716,43 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="G6:AD6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:AD4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:AD5"/>
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:AD2"/>
@@ -5723,43 +5760,6 @@
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="L3:AD3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:AD4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:AD5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="G6:AD6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.70972222222222203" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
merge activities in tidsplan
</commit_message>
<xml_diff>
--- a/doc/projektplan/05Tidplan01.xlsx
+++ b/doc/projektplan/05Tidplan01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,265 +13,252 @@
     <sheet name="Summering TID" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
-  <si>
-    <t>PLANERING</t>
-  </si>
-  <si>
-    <t>Projekt:</t>
-  </si>
-  <si>
-    <t>Projektgrupp:</t>
-  </si>
-  <si>
-    <t>Datum: 2018-09-26</t>
-  </si>
-  <si>
-    <t>Granskad:</t>
-  </si>
-  <si>
-    <t>Beställare: Mattias Krysander</t>
-  </si>
-  <si>
-    <t>Version: 0.1</t>
-  </si>
-  <si>
-    <t>NH, EH, YH</t>
-  </si>
-  <si>
-    <t>Kurs: TSEA29</t>
-  </si>
-  <si>
-    <t>Utfärdare: Jakob Arvidsson</t>
-  </si>
-  <si>
-    <t>OLIKA FASER</t>
-  </si>
-  <si>
-    <t>TID</t>
-  </si>
-  <si>
-    <t>VEM</t>
-  </si>
-  <si>
-    <t>TIDPLAN (när), veckonummer</t>
-  </si>
-  <si>
-    <t>Nr</t>
-  </si>
-  <si>
-    <t>Beskrivning</t>
-  </si>
-  <si>
-    <t>Timmar</t>
-  </si>
-  <si>
-    <t>Initialer</t>
-  </si>
-  <si>
-    <t>Totalt</t>
-  </si>
-  <si>
-    <t>Alla</t>
-  </si>
-  <si>
-    <t>Designfas (v40 – v45)</t>
-  </si>
-  <si>
-    <t>Utförandefas (v46 – v50)</t>
-  </si>
-  <si>
-    <t>DESIGNFAS</t>
-  </si>
-  <si>
-    <t>Skriva rapport</t>
-  </si>
-  <si>
-    <t>Rita blockdiagram</t>
-  </si>
-  <si>
-    <t>Rita kretsscheman</t>
-  </si>
-  <si>
-    <t>Systemdesign</t>
-  </si>
-  <si>
-    <t>Hårdvarudesign</t>
-  </si>
-  <si>
-    <t>Mjukvarudesign</t>
-  </si>
-  <si>
-    <t>Tidsrapport</t>
-  </si>
-  <si>
-    <t>Utbildning</t>
-  </si>
-  <si>
-    <t>Möten</t>
-  </si>
-  <si>
-    <t>Buffer</t>
-  </si>
-  <si>
-    <t>UTFÖRANDEFAS</t>
-  </si>
-  <si>
-    <t>Koppla och installera</t>
-  </si>
-  <si>
-    <t>Implementera mjukvarubaser</t>
-  </si>
-  <si>
-    <t>Kameran tillåter bildbearbeting</t>
-  </si>
-  <si>
-    <t>Skicka och ta emot fjärrstyrningskommandon</t>
-  </si>
-  <si>
-    <t>Upptäcka kanter I bilder</t>
-  </si>
-  <si>
-    <t>Upptäcka linjer</t>
-  </si>
-  <si>
-    <t>Transformera 3D-perspektiv till en ortograsik 2D-bild sedd uppifrån</t>
-  </si>
-  <si>
-    <t>Avgör felvärde, beräkna det från 2D kartan</t>
-  </si>
-  <si>
-    <t>Tolka karta</t>
-  </si>
-  <si>
-    <t>Hitta kortaste väg</t>
-  </si>
-  <si>
-    <t>Köra genom rondell</t>
-  </si>
-  <si>
-    <t>Avgör position</t>
-  </si>
-  <si>
-    <t>Reglera styrning utefter felvärde och följ vägfiler</t>
-  </si>
-  <si>
-    <t>Navigera till bestämd stopplinje</t>
-  </si>
-  <si>
-    <t>Parkera I stoppficka vid stopplinje</t>
-  </si>
-  <si>
-    <t>Upptäcka hinder och stanna för det</t>
-  </si>
-  <si>
-    <t>Aktivera motor</t>
-  </si>
-  <si>
-    <t>Hantera svängningar</t>
-  </si>
-  <si>
-    <t>Broms</t>
-  </si>
-  <si>
-    <t>3D-utskrifter, fästen</t>
-  </si>
-  <si>
-    <t>Filtrering av brus från analoga sensorer</t>
-  </si>
-  <si>
-    <t>Konvertera sensorvärden till SI-enheter</t>
-  </si>
-  <si>
-    <t>Skicka värden till kommunikationsmodulen</t>
-  </si>
-  <si>
-    <t>Visa utvalda värden på LCD-display</t>
-  </si>
-  <si>
-    <t>Kör och styr taxin från gränssnittet</t>
-  </si>
-  <si>
-    <t>Mata in konstantparameter under körning</t>
-  </si>
-  <si>
-    <t>Visa upp mätdata från taxin</t>
-  </si>
-  <si>
-    <t>Mata in en karta av banan</t>
-  </si>
-  <si>
-    <t>Rita en karta på gränssnittet med nuvarande taxins position markerad</t>
-  </si>
-  <si>
-    <t>Trådlös länk</t>
-  </si>
-  <si>
-    <t>Kommunikation sensormodul</t>
-  </si>
-  <si>
-    <t>Kommunikation styrmodul</t>
-  </si>
-  <si>
-    <t>Unit-tester</t>
-  </si>
-  <si>
-    <t>Integrationstester</t>
-  </si>
-  <si>
-    <t>Sytemtestning</t>
-  </si>
-  <si>
-    <t>Teknisk dokumentation</t>
-  </si>
-  <si>
-    <t>Efterstudie</t>
-  </si>
-  <si>
-    <t>Användarmanual</t>
-  </si>
-  <si>
-    <t>Statusrapport</t>
-  </si>
-  <si>
-    <t>JA</t>
-  </si>
-  <si>
-    <t>Summa antal timmar:</t>
-  </si>
-  <si>
-    <t>SUMMERING AV TID</t>
-  </si>
-  <si>
-    <t>Datum:</t>
-  </si>
-  <si>
-    <t>Beställare:</t>
-  </si>
-  <si>
-    <t>Utfärdare:</t>
-  </si>
-  <si>
-    <t>Kurs:</t>
-  </si>
-  <si>
-    <t>RESURS</t>
-  </si>
-  <si>
-    <t>NEDLAGD TID (per vecka)</t>
-  </si>
-  <si>
-    <t>Namn</t>
-  </si>
-  <si>
-    <t>Sa</t>
-  </si>
-  <si>
-    <t>Summa antal timmar:  </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
+  <si>
+    <t xml:space="preserve">PLANERING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projekt:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projektgrupp:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datum: 2018-09-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granskad:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beställare: Mattias Krysander</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version: 0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH, EH, YH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurs: TSEA29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utfärdare: Jakob Arvidsson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLIKA FASER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIDPLAN (när), veckonummer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beskrivning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initialer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Totalt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designfas (v40 – v45)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utförandefas (v46 – v50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESIGNFAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systemdesign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hårdvarudesign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mjukvarudesign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dokument</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rita blockdiagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rita kretsscheman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Möten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTFÖRANDEFAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allmänt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koppla och installera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementera mjukvarubaser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommunikationsmodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mjukvara för kommunikationsmodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bildbearbetning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upptäcka kanter I bilder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upptäcka linjer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transformera 3D-perspektiv till en ortograsik 2D-bild sedd uppifrån</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avgör felvärde, beräkna det från 2D kartan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autonom körning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Position i karta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hitta kortaste säkra väg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reglera styrning utefter felvärde och följ vägfiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigera till bestämd stopplinje/parkeringsficka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Styrmodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driva bilen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensormodul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bearbeta sensorvärden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skicka ut värden till andra moduler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Användargränssnitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kör och styr taxin från gränssnittet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inmatning till gränssnitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visa info på gränssnitt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anslutningar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trådlös länk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit-tester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrationstester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sytemtestning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teknisk dokumentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efterstudie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Användarmanual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diverse rapporter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summa antal timmar:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUMMERING AV TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datum:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beställare:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utfärdare:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kurs:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESURS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEDLAGD TID (per vecka)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Namn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summa antal timmar:  </t>
   </si>
 </sst>
 </file>
@@ -279,7 +266,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="14">
@@ -739,16 +726,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -931,11 +918,11 @@
   <dxfs count="2">
     <dxf>
       <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF9C0006"/>
         <sz val="10"/>
-        <color rgb="FF9C0006"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -945,11 +932,11 @@
     </dxf>
     <dxf>
       <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF006100"/>
         <sz val="10"/>
-        <color rgb="FF006100"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -1028,18 +1015,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.73"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1052,25 +1039,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:U70"/>
+  <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y14" activeCellId="0" sqref="Y14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.14285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1428571428571"/>
-    <col collapsed="false" hidden="true" max="3" min="3" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.85714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.56632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2857142857143"/>
-    <col collapsed="false" hidden="false" max="20" min="8" style="0" width="4.42857142857143"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="5.85714285714286"/>
-    <col collapsed="false" hidden="false" max="1014" min="22" style="0" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="11.5714285714286"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="8" style="0" width="4.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="5.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="22" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,9 +1286,7 @@
       <c r="U7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="n">
-        <v>1</v>
-      </c>
+      <c r="A8" s="20"/>
       <c r="B8" s="22" t="s">
         <v>18</v>
       </c>
@@ -1351,9 +1336,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="n">
-        <v>2</v>
-      </c>
+      <c r="A9" s="20"/>
       <c r="B9" s="22" t="s">
         <v>20</v>
       </c>
@@ -1361,7 +1344,7 @@
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="23" t="n">
-        <v>420</v>
+        <v>220</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>19</v>
@@ -1385,9 +1368,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="n">
-        <v>3</v>
-      </c>
+      <c r="A10" s="20"/>
       <c r="B10" s="22" t="s">
         <v>21</v>
       </c>
@@ -1395,7 +1376,7 @@
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="23" t="n">
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="G10" s="23" t="s">
         <v>19</v>
@@ -1507,32 +1488,43 @@
       <c r="U12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="23" t="n">
-        <v>80</v>
-      </c>
-      <c r="G13" s="23" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="29" t="n">
+        <f aca="false">SUM(F14:F16)</f>
+        <v>185</v>
+      </c>
+      <c r="G13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="23" t="n">
-        <v>7</v>
-      </c>
-      <c r="I13" s="23" t="n">
-        <v>19</v>
-      </c>
-      <c r="J13" s="23"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="23" t="n">
-        <v>54</v>
+      <c r="H13" s="18" t="n">
+        <f aca="false">SUM(H14:H16)</f>
+        <v>96</v>
+      </c>
+      <c r="I13" s="18" t="n">
+        <f aca="false">SUM(I14:I16)</f>
+        <v>74</v>
+      </c>
+      <c r="J13" s="18" t="n">
+        <f aca="false">SUM(J14:J16)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="18" t="n">
+        <f aca="false">SUM(K14:K16)</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="18" t="n">
+        <f aca="false">SUM(L14:L16)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="18" t="n">
+        <f aca="false">SUM(M14:M16)</f>
+        <v>15</v>
       </c>
       <c r="N13" s="26"/>
       <c r="O13" s="26"/>
@@ -1541,14 +1533,14 @@
       <c r="R13" s="26"/>
       <c r="S13" s="26"/>
       <c r="T13" s="26"/>
-      <c r="U13" s="21" t="n">
-        <f aca="false">SUM(H13:T13)</f>
-        <v>80</v>
+      <c r="U13" s="18" t="n">
+        <f aca="false">SUM(U14:U16)</f>
+        <v>185</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>24</v>
@@ -1563,7 +1555,7 @@
         <v>19</v>
       </c>
       <c r="H14" s="23" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="I14" s="23" t="n">
         <v>20</v>
@@ -1572,7 +1564,7 @@
       <c r="K14" s="27"/>
       <c r="L14" s="28"/>
       <c r="M14" s="23" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
@@ -1588,7 +1580,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>25</v>
@@ -1597,22 +1589,22 @@
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
       <c r="F15" s="23" t="n">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="23" t="n">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="I15" s="23" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J15" s="23"/>
       <c r="K15" s="27"/>
       <c r="L15" s="28"/>
       <c r="M15" s="23" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="N15" s="26"/>
       <c r="O15" s="26"/>
@@ -1623,12 +1615,12 @@
       <c r="T15" s="26"/>
       <c r="U15" s="21" t="n">
         <f aca="false">SUM(H15:T15)</f>
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>26</v>
@@ -1637,22 +1629,22 @@
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
       <c r="F16" s="23" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="G16" s="23" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="23" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I16" s="23" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J16" s="23"/>
       <c r="K16" s="27"/>
       <c r="L16" s="28"/>
       <c r="M16" s="23" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N16" s="26"/>
       <c r="O16" s="26"/>
@@ -1663,37 +1655,25 @@
       <c r="T16" s="26"/>
       <c r="U16" s="21" t="n">
         <f aca="false">SUM(H16:T16)</f>
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="B17" s="22" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23" t="n">
-        <v>75</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="I17" s="23" t="n">
-        <v>30</v>
-      </c>
-      <c r="J17" s="23"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="23" t="n">
-        <v>5</v>
-      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
@@ -1701,14 +1681,11 @@
       <c r="R17" s="26"/>
       <c r="S17" s="26"/>
       <c r="T17" s="26"/>
-      <c r="U17" s="21" t="n">
-        <f aca="false">SUM(H17:T17)</f>
-        <v>75</v>
-      </c>
+      <c r="U17" s="18"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>28</v>
@@ -1717,22 +1694,22 @@
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="23" t="n">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="G18" s="23" t="s">
         <v>19</v>
       </c>
       <c r="H18" s="23" t="n">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="I18" s="23" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J18" s="23"/>
       <c r="K18" s="27"/>
       <c r="L18" s="28"/>
       <c r="M18" s="23" t="n">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="N18" s="26"/>
       <c r="O18" s="26"/>
@@ -1743,12 +1720,12 @@
       <c r="T18" s="26"/>
       <c r="U18" s="21" t="n">
         <f aca="false">SUM(H18:T18)</f>
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>29</v>
@@ -1757,18 +1734,22 @@
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
       <c r="F19" s="23" t="n">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="G19" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
+      <c r="H19" s="23" t="n">
+        <v>8</v>
+      </c>
+      <c r="I19" s="23" t="n">
+        <v>20</v>
+      </c>
       <c r="J19" s="23"/>
       <c r="K19" s="27"/>
       <c r="L19" s="28"/>
       <c r="M19" s="23" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="N19" s="26"/>
       <c r="O19" s="26"/>
@@ -1779,12 +1760,12 @@
       <c r="T19" s="26"/>
       <c r="U19" s="21" t="n">
         <f aca="false">SUM(H19:T19)</f>
-        <v>3</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>30</v>
@@ -1793,20 +1774,22 @@
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
       <c r="F20" s="23" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="G20" s="23" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="23" t="n">
-        <v>6</v>
-      </c>
-      <c r="I20" s="23"/>
+        <v>9</v>
+      </c>
+      <c r="I20" s="23" t="n">
+        <v>20</v>
+      </c>
       <c r="J20" s="23"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="28"/>
       <c r="M20" s="23" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="N20" s="26"/>
       <c r="O20" s="26"/>
@@ -1817,37 +1800,25 @@
       <c r="T20" s="26"/>
       <c r="U20" s="21" t="n">
         <f aca="false">SUM(H20:T20)</f>
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20" t="n">
-        <v>12</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="23" t="n">
-        <v>21</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="23" t="n">
-        <v>7</v>
-      </c>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23" t="n">
-        <v>7</v>
-      </c>
-      <c r="K21" s="27"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="23" t="n">
-        <v>7</v>
-      </c>
+      <c r="A21" s="20"/>
+      <c r="B21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
       <c r="N21" s="26"/>
       <c r="O21" s="26"/>
       <c r="P21" s="26"/>
@@ -1855,41 +1826,34 @@
       <c r="R21" s="26"/>
       <c r="S21" s="26"/>
       <c r="T21" s="26"/>
-      <c r="U21" s="21" t="n">
-        <f aca="false">SUM(H21:T21)</f>
-        <v>21</v>
-      </c>
+      <c r="U21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="20" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
       <c r="F22" s="23" t="n">
-        <f aca="false">(420-SUM(F13:F21))</f>
         <v>21</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="23" t="n">
-        <f aca="false">(140-SUM(H13:H21))</f>
         <v>7</v>
       </c>
-      <c r="I22" s="23" t="n">
-        <f aca="false">(140-SUM(I13:I21))</f>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23" t="n">
         <v>7</v>
       </c>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="28"/>
       <c r="M22" s="23" t="n">
-        <f aca="false">(133-SUM(M13:M21))</f>
         <v>7</v>
       </c>
       <c r="N22" s="26"/>
@@ -1906,44 +1870,35 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="20" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
       <c r="F23" s="23" t="n">
-        <f aca="false">SUM(F13:F22)</f>
-        <v>420</v>
+        <f aca="false">(420-SUM(F18:F22))</f>
+        <v>226</v>
       </c>
       <c r="G23" s="23" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="23" t="n">
-        <f aca="false">SUM(H13:H22)</f>
-        <v>140</v>
+        <f aca="false">(140-SUM(H18:H22))</f>
+        <v>109</v>
       </c>
       <c r="I23" s="23" t="n">
-        <f aca="false">SUM(I13:I22)</f>
-        <v>140</v>
-      </c>
-      <c r="J23" s="23" t="n">
-        <f aca="false">SUM(J13:J22)</f>
-        <v>7</v>
-      </c>
-      <c r="K23" s="23" t="n">
-        <f aca="false">SUM(K13:K22)</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="23" t="n">
-        <f aca="false">SUM(L13:L22)</f>
-        <v>0</v>
-      </c>
+        <f aca="false">(140-SUM(I18:I22))</f>
+        <v>81</v>
+      </c>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
       <c r="M23" s="23" t="n">
-        <f aca="false">SUM(M13:M22)</f>
-        <v>133</v>
+        <f aca="false">(133-SUM(M18:M22))</f>
+        <v>36</v>
       </c>
       <c r="N23" s="26"/>
       <c r="O23" s="26"/>
@@ -1954,187 +1909,187 @@
       <c r="T23" s="26"/>
       <c r="U23" s="21" t="n">
         <f aca="false">SUM(H23:T23)</f>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="20" t="n">
+        <v>12</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23" t="n">
+        <f aca="false">SUM(F18:F23)</f>
         <v>420</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="s">
+      <c r="G24" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="23" t="n">
+        <f aca="false">SUM(H18:H23)</f>
+        <v>140</v>
+      </c>
+      <c r="I24" s="23" t="n">
+        <f aca="false">SUM(I18:I23)</f>
+        <v>140</v>
+      </c>
+      <c r="J24" s="23" t="n">
+        <f aca="false">SUM(J18:J23)</f>
+        <v>7</v>
+      </c>
+      <c r="K24" s="23" t="n">
+        <f aca="false">SUM(K18:K23)</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="23" t="n">
+        <f aca="false">SUM(L18:L23)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="23" t="n">
+        <f aca="false">SUM(M18:M23)</f>
+        <v>133</v>
+      </c>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="26"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="26"/>
+      <c r="U24" s="21" t="n">
+        <f aca="false">SUM(H24:T24)</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16" t="s">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="G25" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H25" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="16"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18" t="s">
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B26" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="18" t="s">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G26" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="20" t="n">
+      <c r="H26" s="20" t="n">
         <v>40</v>
       </c>
-      <c r="I25" s="20" t="n">
+      <c r="I26" s="20" t="n">
         <v>41</v>
       </c>
-      <c r="J25" s="20" t="n">
+      <c r="J26" s="20" t="n">
         <v>42</v>
       </c>
-      <c r="K25" s="20" t="n">
+      <c r="K26" s="20" t="n">
         <v>43</v>
       </c>
-      <c r="L25" s="20" t="n">
+      <c r="L26" s="20" t="n">
         <v>44</v>
       </c>
-      <c r="M25" s="20" t="n">
+      <c r="M26" s="20" t="n">
         <v>45</v>
       </c>
-      <c r="N25" s="20" t="n">
+      <c r="N26" s="20" t="n">
         <v>46</v>
       </c>
-      <c r="O25" s="20" t="n">
+      <c r="O26" s="20" t="n">
         <v>47</v>
       </c>
-      <c r="P25" s="20" t="n">
+      <c r="P26" s="20" t="n">
         <v>48</v>
       </c>
-      <c r="Q25" s="20" t="n">
+      <c r="Q26" s="20" t="n">
         <v>49</v>
       </c>
-      <c r="R25" s="20" t="n">
+      <c r="R26" s="20" t="n">
         <v>50</v>
       </c>
-      <c r="S25" s="20" t="n">
+      <c r="S26" s="20" t="n">
         <v>51</v>
       </c>
-      <c r="T25" s="20" t="n">
+      <c r="T26" s="20" t="n">
         <v>52</v>
       </c>
-      <c r="U25" s="21"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="20" t="n">
-        <v>15</v>
-      </c>
-      <c r="B26" s="22" t="s">
+      <c r="U26" s="21"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="20"/>
+      <c r="B27" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="23" t="n">
-        <v>50</v>
-      </c>
-      <c r="G26" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="23" t="n">
-        <v>35</v>
-      </c>
-      <c r="O26" s="23" t="n">
-        <v>10</v>
-      </c>
-      <c r="P26" s="23" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="26"/>
-      <c r="T26" s="26"/>
-      <c r="U26" s="21" t="n">
-        <f aca="false">SUM(H26:R26)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="20" t="n">
-        <v>16</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="23" t="n">
-        <v>60</v>
-      </c>
-      <c r="G27" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
       <c r="J27" s="26"/>
       <c r="K27" s="26"/>
       <c r="L27" s="26"/>
       <c r="M27" s="26"/>
-      <c r="N27" s="23" t="n">
-        <v>40</v>
-      </c>
-      <c r="O27" s="23" t="n">
-        <v>20</v>
-      </c>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="23"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
       <c r="S27" s="26"/>
       <c r="T27" s="26"/>
-      <c r="U27" s="21" t="n">
-        <f aca="false">SUM(H27:R27)</f>
-        <v>60</v>
-      </c>
+      <c r="U27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20" t="n">
-        <v>17</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="30" t="n">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23" t="n">
+        <v>55</v>
       </c>
       <c r="G28" s="23" t="s">
         <v>19</v>
@@ -2145,34 +2100,36 @@
       <c r="K28" s="26"/>
       <c r="L28" s="26"/>
       <c r="M28" s="26"/>
-      <c r="N28" s="30"/>
-      <c r="O28" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="P28" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
+      <c r="N28" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="O28" s="23" t="n">
+        <v>10</v>
+      </c>
+      <c r="P28" s="23" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
       <c r="S28" s="26"/>
       <c r="T28" s="26"/>
       <c r="U28" s="21" t="n">
         <f aca="false">SUM(H28:R28)</f>
-        <v>8</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="20" t="n">
-        <v>18</v>
-      </c>
-      <c r="B29" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="30" t="n">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="23" t="n">
+        <v>60</v>
       </c>
       <c r="G29" s="23" t="s">
         <v>19</v>
@@ -2183,67 +2140,61 @@
       <c r="K29" s="26"/>
       <c r="L29" s="26"/>
       <c r="M29" s="26"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="P29" s="30"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
+      <c r="N29" s="23" t="n">
+        <v>40</v>
+      </c>
+      <c r="O29" s="23" t="n">
+        <v>20</v>
+      </c>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
+      <c r="R29" s="23"/>
       <c r="S29" s="26"/>
       <c r="T29" s="26"/>
       <c r="U29" s="21" t="n">
         <f aca="false">SUM(H29:R29)</f>
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B30" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="30" t="n">
-        <v>15</v>
-      </c>
-      <c r="G30" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="A30" s="20"/>
+      <c r="B30" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
       <c r="J30" s="26"/>
       <c r="K30" s="26"/>
       <c r="L30" s="26"/>
       <c r="M30" s="26"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="30" t="n">
-        <v>15</v>
-      </c>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
+      <c r="Q30" s="23"/>
+      <c r="R30" s="23"/>
       <c r="S30" s="26"/>
       <c r="T30" s="26"/>
-      <c r="U30" s="21" t="n">
-        <f aca="false">SUM(H30:R30)</f>
-        <v>15</v>
+      <c r="U30" s="29" t="n">
+        <f aca="false">SUM(U31:U34)</f>
+        <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20" t="n">
-        <v>20</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30" t="n">
+        <v>15</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="31" t="n">
         <v>15</v>
       </c>
       <c r="G31" s="23" t="s">
@@ -2255,13 +2206,15 @@
       <c r="K31" s="26"/>
       <c r="L31" s="26"/>
       <c r="M31" s="26"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="P31" s="31" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="31"/>
       <c r="S31" s="26"/>
       <c r="T31" s="26"/>
       <c r="U31" s="21" t="n">
@@ -2270,54 +2223,41 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="20" t="n">
-        <v>21</v>
-      </c>
-      <c r="B32" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30" t="n">
-        <v>15</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="A32" s="20"/>
+      <c r="B32" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
       <c r="J32" s="26"/>
       <c r="K32" s="26"/>
       <c r="L32" s="26"/>
       <c r="M32" s="26"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q32" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="R32" s="30"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
+      <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
       <c r="S32" s="26"/>
       <c r="T32" s="26"/>
-      <c r="U32" s="21" t="n">
-        <f aca="false">SUM(H32:R32)</f>
-        <v>15</v>
-      </c>
+      <c r="U32" s="29"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="20" t="n">
-        <v>22</v>
-      </c>
-      <c r="B33" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="30" t="n">
+        <v>16</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="31" t="n">
         <v>15</v>
       </c>
       <c r="G33" s="23" t="s">
@@ -2329,13 +2269,13 @@
       <c r="K33" s="26"/>
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
-      <c r="N33" s="30"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30" t="n">
+      <c r="N33" s="31"/>
+      <c r="O33" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="R33" s="30"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="31"/>
+      <c r="R33" s="31"/>
       <c r="S33" s="26"/>
       <c r="T33" s="26"/>
       <c r="U33" s="21" t="n">
@@ -2345,16 +2285,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20" t="n">
-        <v>23</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="30" t="n">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="31" t="n">
+        <v>15</v>
       </c>
       <c r="G34" s="23" t="s">
         <v>19</v>
@@ -2365,34 +2305,32 @@
       <c r="K34" s="26"/>
       <c r="L34" s="26"/>
       <c r="M34" s="26"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q34" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="R34" s="30"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="31" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="31"/>
       <c r="S34" s="26"/>
       <c r="T34" s="26"/>
       <c r="U34" s="21" t="n">
         <f aca="false">SUM(H34:R34)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="20" t="n">
-        <v>24</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30" t="n">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="31" t="n">
+        <v>15</v>
       </c>
       <c r="G35" s="23" t="s">
         <v>19</v>
@@ -2403,32 +2341,34 @@
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
       <c r="M35" s="26"/>
-      <c r="N35" s="30"/>
-      <c r="O35" s="30"/>
-      <c r="P35" s="30"/>
-      <c r="Q35" s="30"/>
-      <c r="R35" s="30" t="n">
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q35" s="31" t="n">
         <v>10</v>
       </c>
+      <c r="R35" s="31"/>
       <c r="S35" s="26"/>
       <c r="T35" s="26"/>
       <c r="U35" s="21" t="n">
         <f aca="false">SUM(H35:R35)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="20" t="n">
-        <v>25</v>
-      </c>
-      <c r="B36" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="30" t="n">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="31" t="n">
+        <v>15</v>
       </c>
       <c r="G36" s="23" t="s">
         <v>19</v>
@@ -2439,70 +2379,57 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30" t="n">
-        <v>10</v>
-      </c>
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="31"/>
+      <c r="Q36" s="31" t="n">
+        <v>15</v>
+      </c>
+      <c r="R36" s="31"/>
       <c r="S36" s="26"/>
       <c r="T36" s="26"/>
       <c r="U36" s="21" t="n">
         <f aca="false">SUM(H36:R36)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="20" t="n">
-        <v>26</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="30" t="n">
-        <v>8</v>
-      </c>
-      <c r="G37" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="A37" s="20"/>
+      <c r="B37" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
       <c r="J37" s="26"/>
       <c r="K37" s="26"/>
       <c r="L37" s="26"/>
       <c r="M37" s="26"/>
-      <c r="N37" s="30"/>
-      <c r="O37" s="30"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="R37" s="30" t="n">
-        <v>4</v>
-      </c>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
       <c r="S37" s="26"/>
       <c r="T37" s="26"/>
-      <c r="U37" s="21" t="n">
-        <f aca="false">SUM(H37:R37)</f>
-        <v>8</v>
-      </c>
+      <c r="U37" s="29"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="20" t="n">
-        <v>27</v>
-      </c>
-      <c r="B38" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="30" t="n">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="31" t="n">
+        <v>18</v>
       </c>
       <c r="G38" s="23" t="s">
         <v>19</v>
@@ -2513,32 +2440,36 @@
       <c r="K38" s="26"/>
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
-      <c r="N38" s="30"/>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="R38" s="30"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q38" s="31" t="n">
+        <v>9</v>
+      </c>
+      <c r="R38" s="31" t="n">
+        <v>4</v>
+      </c>
       <c r="S38" s="26"/>
       <c r="T38" s="26"/>
       <c r="U38" s="21" t="n">
         <f aca="false">SUM(H38:R38)</f>
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="20" t="n">
-        <v>29</v>
-      </c>
-      <c r="B39" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="30" t="n">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="31" t="n">
+        <v>18</v>
       </c>
       <c r="G39" s="23" t="s">
         <v>19</v>
@@ -2549,32 +2480,32 @@
       <c r="K39" s="26"/>
       <c r="L39" s="26"/>
       <c r="M39" s="26"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30" t="n">
-        <v>20</v>
-      </c>
-      <c r="R39" s="30"/>
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31"/>
+      <c r="R39" s="31" t="n">
+        <v>18</v>
+      </c>
       <c r="S39" s="26"/>
       <c r="T39" s="26"/>
       <c r="U39" s="21" t="n">
         <f aca="false">SUM(H39:R39)</f>
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="20" t="n">
-        <v>30</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="30" t="n">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="31" t="n">
+        <v>20</v>
       </c>
       <c r="G40" s="23" t="s">
         <v>19</v>
@@ -2585,32 +2516,34 @@
       <c r="K40" s="26"/>
       <c r="L40" s="26"/>
       <c r="M40" s="26"/>
-      <c r="N40" s="30"/>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="R40" s="30" t="n">
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31"/>
+      <c r="Q40" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="R40" s="31" t="n">
         <v>10</v>
       </c>
       <c r="S40" s="26"/>
       <c r="T40" s="26"/>
       <c r="U40" s="21" t="n">
         <f aca="false">SUM(H40:R40)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="20" t="n">
-        <v>31</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="30" t="n">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="31" t="n">
+        <v>30</v>
       </c>
       <c r="G41" s="23" t="s">
         <v>19</v>
@@ -2621,68 +2554,59 @@
       <c r="K41" s="26"/>
       <c r="L41" s="26"/>
       <c r="M41" s="26"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30" t="n">
-        <v>8</v>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31" t="n">
+        <v>20</v>
+      </c>
+      <c r="R41" s="31" t="n">
+        <v>10</v>
       </c>
       <c r="S41" s="26"/>
       <c r="T41" s="26"/>
       <c r="U41" s="21" t="n">
         <f aca="false">SUM(H41:R41)</f>
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="20" t="n">
-        <v>32</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="G42" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="A42" s="20"/>
+      <c r="B42" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
       <c r="H42" s="26"/>
       <c r="I42" s="26"/>
       <c r="J42" s="26"/>
       <c r="K42" s="26"/>
       <c r="L42" s="26"/>
       <c r="M42" s="26"/>
-      <c r="N42" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="O42" s="30"/>
-      <c r="P42" s="30"/>
-      <c r="Q42" s="30"/>
-      <c r="R42" s="30"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
       <c r="S42" s="26"/>
       <c r="T42" s="26"/>
-      <c r="U42" s="21" t="n">
-        <f aca="false">SUM(H42:R42)</f>
-        <v>5</v>
-      </c>
+      <c r="U42" s="29"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="20" t="n">
-        <v>33</v>
-      </c>
-      <c r="B43" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="30" t="n">
-        <v>5</v>
+        <v>24</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="31" t="n">
+        <v>15</v>
       </c>
       <c r="G43" s="23" t="s">
         <v>19</v>
@@ -2693,68 +2617,61 @@
       <c r="K43" s="26"/>
       <c r="L43" s="26"/>
       <c r="M43" s="26"/>
-      <c r="N43" s="30"/>
-      <c r="O43" s="30" t="n">
+      <c r="N43" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="30"/>
-      <c r="R43" s="30"/>
+      <c r="O43" s="31" t="n">
+        <v>5</v>
+      </c>
+      <c r="P43" s="31" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q43" s="31"/>
+      <c r="R43" s="31"/>
       <c r="S43" s="26"/>
       <c r="T43" s="26"/>
       <c r="U43" s="21" t="n">
         <f aca="false">SUM(H43:R43)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="20" t="n">
-        <v>34</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="G44" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="A44" s="20"/>
+      <c r="B44" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
       <c r="H44" s="26"/>
       <c r="I44" s="26"/>
       <c r="J44" s="26"/>
       <c r="K44" s="26"/>
       <c r="L44" s="26"/>
       <c r="M44" s="26"/>
-      <c r="N44" s="30"/>
-      <c r="O44" s="30"/>
-      <c r="P44" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q44" s="30"/>
-      <c r="R44" s="30"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
       <c r="S44" s="26"/>
       <c r="T44" s="26"/>
-      <c r="U44" s="21" t="n">
-        <f aca="false">SUM(H44:R44)</f>
-        <v>5</v>
-      </c>
+      <c r="U44" s="29"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="20" t="n">
-        <v>35</v>
-      </c>
-      <c r="B45" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="30" t="n">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="31" t="n">
+        <v>15</v>
       </c>
       <c r="G45" s="23" t="s">
         <v>19</v>
@@ -2765,32 +2682,34 @@
       <c r="K45" s="26"/>
       <c r="L45" s="26"/>
       <c r="M45" s="26"/>
-      <c r="N45" s="30" t="n">
+      <c r="N45" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="O45" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="O45" s="30"/>
-      <c r="P45" s="30"/>
-      <c r="Q45" s="30"/>
-      <c r="R45" s="30"/>
+      <c r="P45" s="31"/>
+      <c r="Q45" s="31"/>
+      <c r="R45" s="31"/>
       <c r="S45" s="26"/>
       <c r="T45" s="26"/>
       <c r="U45" s="21" t="n">
         <f aca="false">SUM(H45:R45)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="20" t="n">
-        <v>36</v>
-      </c>
-      <c r="B46" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="30" t="n">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="31" t="n">
+        <v>18</v>
       </c>
       <c r="G46" s="23" t="s">
         <v>19</v>
@@ -2801,70 +2720,61 @@
       <c r="K46" s="26"/>
       <c r="L46" s="26"/>
       <c r="M46" s="26"/>
-      <c r="N46" s="30" t="n">
+      <c r="N46" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="O46" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="P46" s="30"/>
-      <c r="Q46" s="30"/>
-      <c r="R46" s="30"/>
+      <c r="O46" s="31" t="n">
+        <v>9</v>
+      </c>
+      <c r="P46" s="31" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="31"/>
       <c r="S46" s="26"/>
       <c r="T46" s="26"/>
       <c r="U46" s="21" t="n">
         <f aca="false">SUM(H46:R46)</f>
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="20" t="n">
-        <v>37</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="G47" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="A47" s="20"/>
+      <c r="B47" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
       <c r="H47" s="26"/>
       <c r="I47" s="26"/>
       <c r="J47" s="26"/>
       <c r="K47" s="26"/>
       <c r="L47" s="26"/>
       <c r="M47" s="26"/>
-      <c r="N47" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="O47" s="30"/>
-      <c r="P47" s="30"/>
-      <c r="Q47" s="30"/>
-      <c r="R47" s="30"/>
+      <c r="N47" s="29"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="29"/>
+      <c r="Q47" s="29"/>
+      <c r="R47" s="29"/>
       <c r="S47" s="26"/>
       <c r="T47" s="26"/>
-      <c r="U47" s="21" t="n">
-        <f aca="false">SUM(H47:R47)</f>
-        <v>5</v>
-      </c>
+      <c r="U47" s="29"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="20" t="n">
-        <v>38</v>
-      </c>
-      <c r="B48" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="30" t="n">
-        <v>10</v>
+        <v>27</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="31" t="n">
+        <v>15</v>
       </c>
       <c r="G48" s="23" t="s">
         <v>19</v>
@@ -2875,34 +2785,36 @@
       <c r="K48" s="26"/>
       <c r="L48" s="26"/>
       <c r="M48" s="26"/>
-      <c r="N48" s="30" t="n">
+      <c r="N48" s="31" t="n">
+        <v>6</v>
+      </c>
+      <c r="O48" s="31" t="n">
+        <v>4</v>
+      </c>
+      <c r="P48" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="O48" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="P48" s="30"/>
-      <c r="Q48" s="30"/>
-      <c r="R48" s="30"/>
+      <c r="Q48" s="31"/>
+      <c r="R48" s="31"/>
       <c r="S48" s="26"/>
       <c r="T48" s="26"/>
       <c r="U48" s="21" t="n">
         <f aca="false">SUM(H48:R48)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="20" t="n">
-        <v>39</v>
-      </c>
-      <c r="B49" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="30" t="n">
-        <v>8</v>
+        <v>28</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="31" t="n">
+        <v>15</v>
       </c>
       <c r="G49" s="23" t="s">
         <v>19</v>
@@ -2913,34 +2825,32 @@
       <c r="K49" s="26"/>
       <c r="L49" s="26"/>
       <c r="M49" s="26"/>
-      <c r="N49" s="30"/>
-      <c r="O49" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="P49" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q49" s="30"/>
-      <c r="R49" s="30"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q49" s="31"/>
+      <c r="R49" s="31"/>
       <c r="S49" s="26"/>
       <c r="T49" s="26"/>
       <c r="U49" s="21" t="n">
         <f aca="false">SUM(H49:R49)</f>
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="20" t="n">
-        <v>40</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="30" t="n">
-        <v>10</v>
+        <v>29</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="31" t="n">
+        <v>15</v>
       </c>
       <c r="G50" s="23" t="s">
         <v>19</v>
@@ -2951,70 +2861,57 @@
       <c r="K50" s="26"/>
       <c r="L50" s="26"/>
       <c r="M50" s="26"/>
-      <c r="N50" s="30" t="n">
-        <v>6</v>
-      </c>
-      <c r="O50" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="P50" s="30"/>
-      <c r="Q50" s="30"/>
-      <c r="R50" s="30"/>
+      <c r="N50" s="31"/>
+      <c r="O50" s="31"/>
+      <c r="P50" s="31" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q50" s="31"/>
+      <c r="R50" s="31"/>
       <c r="S50" s="26"/>
       <c r="T50" s="26"/>
       <c r="U50" s="21" t="n">
         <f aca="false">SUM(H50:R50)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="20" t="n">
-        <v>41</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="G51" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="A51" s="20"/>
+      <c r="B51" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
       <c r="H51" s="26"/>
       <c r="I51" s="26"/>
       <c r="J51" s="26"/>
       <c r="K51" s="26"/>
       <c r="L51" s="26"/>
       <c r="M51" s="26"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="30"/>
-      <c r="P51" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q51" s="30"/>
-      <c r="R51" s="30"/>
+      <c r="N51" s="29"/>
+      <c r="O51" s="29"/>
+      <c r="P51" s="29"/>
+      <c r="Q51" s="29"/>
+      <c r="R51" s="29"/>
       <c r="S51" s="26"/>
       <c r="T51" s="26"/>
-      <c r="U51" s="21" t="n">
-        <f aca="false">SUM(H51:R51)</f>
-        <v>5</v>
-      </c>
+      <c r="U51" s="29"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="20" t="n">
-        <v>42</v>
-      </c>
-      <c r="B52" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="30" t="n">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="31" t="n">
+        <v>40</v>
       </c>
       <c r="G52" s="23" t="s">
         <v>19</v>
@@ -3025,68 +2922,61 @@
       <c r="K52" s="26"/>
       <c r="L52" s="26"/>
       <c r="M52" s="26"/>
-      <c r="N52" s="30"/>
-      <c r="O52" s="30"/>
-      <c r="P52" s="30" t="n">
+      <c r="N52" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="Q52" s="30"/>
-      <c r="R52" s="30"/>
+      <c r="O52" s="31" t="n">
+        <v>25</v>
+      </c>
+      <c r="P52" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q52" s="31"/>
+      <c r="R52" s="31"/>
       <c r="S52" s="26"/>
       <c r="T52" s="26"/>
       <c r="U52" s="21" t="n">
         <f aca="false">SUM(H52:R52)</f>
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="20" t="n">
-        <v>43</v>
-      </c>
-      <c r="B53" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="G53" s="23" t="s">
-        <v>19</v>
-      </c>
+      <c r="A53" s="20"/>
+      <c r="B53" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
       <c r="H53" s="26"/>
       <c r="I53" s="26"/>
       <c r="J53" s="26"/>
       <c r="K53" s="26"/>
       <c r="L53" s="26"/>
       <c r="M53" s="26"/>
-      <c r="N53" s="30"/>
-      <c r="O53" s="30"/>
-      <c r="P53" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q53" s="30"/>
-      <c r="R53" s="30"/>
+      <c r="N53" s="29"/>
+      <c r="O53" s="29"/>
+      <c r="P53" s="29"/>
+      <c r="Q53" s="29"/>
+      <c r="R53" s="29"/>
       <c r="S53" s="26"/>
       <c r="T53" s="26"/>
-      <c r="U53" s="21" t="n">
-        <f aca="false">SUM(H53:R53)</f>
-        <v>10</v>
-      </c>
+      <c r="U53" s="29"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="20" t="n">
-        <v>44</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="30" t="n">
-        <v>10</v>
+        <v>31</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="31" t="n">
+        <v>40</v>
       </c>
       <c r="G54" s="23" t="s">
         <v>19</v>
@@ -3097,32 +2987,38 @@
       <c r="K54" s="26"/>
       <c r="L54" s="26"/>
       <c r="M54" s="26"/>
-      <c r="N54" s="30"/>
-      <c r="O54" s="30"/>
-      <c r="P54" s="30" t="n">
+      <c r="N54" s="31"/>
+      <c r="O54" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="Q54" s="30"/>
-      <c r="R54" s="30"/>
+      <c r="P54" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q54" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="R54" s="31" t="n">
+        <v>10</v>
+      </c>
       <c r="S54" s="26"/>
       <c r="T54" s="26"/>
       <c r="U54" s="21" t="n">
         <f aca="false">SUM(H54:R54)</f>
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="20" t="n">
-        <v>45</v>
-      </c>
-      <c r="B55" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="30" t="n">
-        <v>10</v>
+        <v>32</v>
+      </c>
+      <c r="B55" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="31" t="n">
+        <v>30</v>
       </c>
       <c r="G55" s="23" t="s">
         <v>19</v>
@@ -3133,34 +3029,36 @@
       <c r="K55" s="26"/>
       <c r="L55" s="26"/>
       <c r="M55" s="26"/>
-      <c r="N55" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="O55" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="P55" s="30"/>
-      <c r="Q55" s="30"/>
-      <c r="R55" s="30"/>
+      <c r="N55" s="31"/>
+      <c r="O55" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="P55" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q55" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="R55" s="31"/>
       <c r="S55" s="26"/>
       <c r="T55" s="26"/>
       <c r="U55" s="21" t="n">
         <f aca="false">SUM(H55:R55)</f>
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="20" t="n">
-        <v>46</v>
-      </c>
-      <c r="B56" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="30" t="n">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="B56" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="31" t="n">
+        <v>30</v>
       </c>
       <c r="G56" s="23" t="s">
         <v>19</v>
@@ -3171,72 +3069,61 @@
       <c r="K56" s="26"/>
       <c r="L56" s="26"/>
       <c r="M56" s="26"/>
-      <c r="N56" s="30"/>
-      <c r="O56" s="30" t="n">
+      <c r="N56" s="31"/>
+      <c r="O56" s="31"/>
+      <c r="P56" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="P56" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q56" s="30"/>
-      <c r="R56" s="30"/>
+      <c r="Q56" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="R56" s="31" t="n">
+        <v>10</v>
+      </c>
       <c r="S56" s="26"/>
       <c r="T56" s="26"/>
       <c r="U56" s="21" t="n">
         <f aca="false">SUM(H56:R56)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="20" t="n">
-        <v>47</v>
-      </c>
-      <c r="B57" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="30" t="n">
-        <v>15</v>
-      </c>
-      <c r="G57" s="23" t="s">
-        <v>19</v>
-      </c>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="20"/>
+      <c r="B57" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
       <c r="H57" s="26"/>
       <c r="I57" s="26"/>
       <c r="J57" s="26"/>
       <c r="K57" s="26"/>
       <c r="L57" s="26"/>
       <c r="M57" s="26"/>
-      <c r="N57" s="30"/>
-      <c r="O57" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="P57" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q57" s="30"/>
-      <c r="R57" s="30"/>
+      <c r="N57" s="29"/>
+      <c r="O57" s="29"/>
+      <c r="P57" s="29"/>
+      <c r="Q57" s="29"/>
+      <c r="R57" s="29"/>
       <c r="S57" s="26"/>
       <c r="T57" s="26"/>
-      <c r="U57" s="21" t="n">
-        <f aca="false">SUM(H57:R57)</f>
-        <v>15</v>
-      </c>
+      <c r="U57" s="29"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="20" t="n">
-        <v>48</v>
-      </c>
-      <c r="B58" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="30" t="n">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="B58" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="31" t="n">
+        <v>50</v>
       </c>
       <c r="G58" s="23" t="s">
         <v>19</v>
@@ -3247,38 +3134,36 @@
       <c r="K58" s="26"/>
       <c r="L58" s="26"/>
       <c r="M58" s="26"/>
-      <c r="N58" s="30"/>
-      <c r="O58" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="P58" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q58" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="R58" s="30" t="n">
-        <v>10</v>
+      <c r="N58" s="31"/>
+      <c r="O58" s="31"/>
+      <c r="P58" s="31" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q58" s="31" t="n">
+        <v>20</v>
+      </c>
+      <c r="R58" s="31" t="n">
+        <v>25</v>
       </c>
       <c r="S58" s="26"/>
       <c r="T58" s="26"/>
       <c r="U58" s="21" t="n">
         <f aca="false">SUM(H58:R58)</f>
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="20" t="n">
-        <v>49</v>
-      </c>
-      <c r="B59" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="30" t="n">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="B59" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="31" t="n">
+        <v>20</v>
       </c>
       <c r="G59" s="23" t="s">
         <v>19</v>
@@ -3289,36 +3174,34 @@
       <c r="K59" s="26"/>
       <c r="L59" s="26"/>
       <c r="M59" s="26"/>
-      <c r="N59" s="30"/>
-      <c r="O59" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="P59" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q59" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="R59" s="30"/>
+      <c r="N59" s="31"/>
+      <c r="O59" s="31"/>
+      <c r="P59" s="31"/>
+      <c r="Q59" s="31" t="n">
+        <v>5</v>
+      </c>
+      <c r="R59" s="31" t="n">
+        <v>15</v>
+      </c>
       <c r="S59" s="26"/>
       <c r="T59" s="26"/>
       <c r="U59" s="21" t="n">
         <f aca="false">SUM(H59:R59)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="20" t="n">
-        <v>50</v>
-      </c>
-      <c r="B60" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="30" t="n">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="31" t="n">
+        <v>20</v>
       </c>
       <c r="G60" s="23" t="s">
         <v>19</v>
@@ -3329,38 +3212,36 @@
       <c r="K60" s="26"/>
       <c r="L60" s="26"/>
       <c r="M60" s="26"/>
-      <c r="N60" s="30"/>
-      <c r="O60" s="30"/>
-      <c r="P60" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q60" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="R60" s="30" t="n">
-        <v>10</v>
+      <c r="N60" s="31"/>
+      <c r="O60" s="31"/>
+      <c r="P60" s="31"/>
+      <c r="Q60" s="31" t="n">
+        <v>5</v>
+      </c>
+      <c r="R60" s="31" t="n">
+        <v>15</v>
       </c>
       <c r="S60" s="26"/>
       <c r="T60" s="26"/>
       <c r="U60" s="21" t="n">
         <f aca="false">SUM(H60:R60)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="20" t="n">
-        <v>51</v>
-      </c>
-      <c r="B61" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C61" s="29"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="30" t="n">
-        <v>50</v>
-      </c>
-      <c r="G61" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B61" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="31" t="n">
+        <v>20</v>
+      </c>
+      <c r="G61" s="31" t="s">
         <v>19</v>
       </c>
       <c r="H61" s="26"/>
@@ -3369,38 +3250,42 @@
       <c r="K61" s="26"/>
       <c r="L61" s="26"/>
       <c r="M61" s="26"/>
-      <c r="N61" s="30"/>
-      <c r="O61" s="30"/>
-      <c r="P61" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="Q61" s="30" t="n">
-        <v>20</v>
-      </c>
-      <c r="R61" s="30" t="n">
-        <v>25</v>
+      <c r="N61" s="31" t="n">
+        <v>4</v>
+      </c>
+      <c r="O61" s="31" t="n">
+        <v>4</v>
+      </c>
+      <c r="P61" s="31" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q61" s="31" t="n">
+        <v>4</v>
+      </c>
+      <c r="R61" s="31" t="n">
+        <v>4</v>
       </c>
       <c r="S61" s="26"/>
       <c r="T61" s="26"/>
       <c r="U61" s="21" t="n">
         <f aca="false">SUM(H61:R61)</f>
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="20" t="n">
-        <v>52</v>
-      </c>
-      <c r="B62" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="30" t="n">
-        <v>20</v>
-      </c>
-      <c r="G62" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="31" t="n">
+        <v>21</v>
+      </c>
+      <c r="G62" s="31" t="s">
         <v>19</v>
       </c>
       <c r="H62" s="26"/>
@@ -3409,36 +3294,39 @@
       <c r="K62" s="26"/>
       <c r="L62" s="26"/>
       <c r="M62" s="26"/>
-      <c r="N62" s="30"/>
-      <c r="O62" s="30"/>
-      <c r="P62" s="30"/>
-      <c r="Q62" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="R62" s="30" t="n">
-        <v>15</v>
+      <c r="N62" s="31" t="n">
+        <v>7</v>
+      </c>
+      <c r="O62" s="31"/>
+      <c r="P62" s="31" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q62" s="31"/>
+      <c r="R62" s="31" t="n">
+        <v>7</v>
       </c>
       <c r="S62" s="26"/>
       <c r="T62" s="26"/>
       <c r="U62" s="21" t="n">
         <f aca="false">SUM(H62:R62)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="20" t="n">
-        <v>53</v>
-      </c>
-      <c r="B63" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" s="29"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="30" t="n">
-        <v>20</v>
-      </c>
-      <c r="G63" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="31" t="n">
+        <f aca="false">(700-SUM(F28:F62))</f>
+        <v>60</v>
+      </c>
+      <c r="G63" s="31" t="s">
         <v>19</v>
       </c>
       <c r="H63" s="26"/>
@@ -3447,361 +3335,173 @@
       <c r="K63" s="26"/>
       <c r="L63" s="26"/>
       <c r="M63" s="26"/>
-      <c r="N63" s="30"/>
-      <c r="O63" s="30"/>
-      <c r="P63" s="30"/>
-      <c r="Q63" s="30" t="n">
+      <c r="N63" s="31" t="n">
+        <f aca="false">(140-SUM(N28:N62))</f>
+        <v>18</v>
+      </c>
+      <c r="O63" s="31" t="n">
+        <f aca="false">(140-SUM(O28:O62))</f>
+        <v>13</v>
+      </c>
+      <c r="P63" s="31" t="n">
+        <f aca="false">(140-SUM(P28:P62))</f>
         <v>5</v>
       </c>
-      <c r="R63" s="30" t="n">
-        <v>15</v>
+      <c r="Q63" s="31" t="n">
+        <f aca="false">(140-SUM(Q28:Q62))</f>
+        <v>12</v>
+      </c>
+      <c r="R63" s="31" t="n">
+        <f aca="false">(140-SUM(R28:R62))</f>
+        <v>12</v>
       </c>
       <c r="S63" s="26"/>
       <c r="T63" s="26"/>
       <c r="U63" s="21" t="n">
         <f aca="false">SUM(H63:R63)</f>
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="20" t="n">
-        <v>54</v>
-      </c>
-      <c r="B64" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="C64" s="29"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="30" t="n">
-        <v>5</v>
-      </c>
-      <c r="G64" s="30" t="s">
-        <v>73</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B64" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="31" t="n">
+        <f aca="false">SUM(F28:F63)</f>
+        <v>700</v>
+      </c>
+      <c r="G64" s="31"/>
       <c r="H64" s="26"/>
       <c r="I64" s="26"/>
       <c r="J64" s="26"/>
       <c r="K64" s="26"/>
       <c r="L64" s="26"/>
       <c r="M64" s="26"/>
-      <c r="N64" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="O64" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="P64" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q64" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="R64" s="30" t="n">
-        <v>1</v>
+      <c r="N64" s="31" t="n">
+        <f aca="false">SUM(N28:N63)</f>
+        <v>140</v>
+      </c>
+      <c r="O64" s="31" t="n">
+        <f aca="false">SUM(O28:O63)</f>
+        <v>140</v>
+      </c>
+      <c r="P64" s="31" t="n">
+        <f aca="false">SUM(P28:P63)</f>
+        <v>140</v>
+      </c>
+      <c r="Q64" s="31" t="n">
+        <f aca="false">SUM(Q28:Q63)</f>
+        <v>140</v>
+      </c>
+      <c r="R64" s="31" t="n">
+        <f aca="false">SUM(R28:R63)</f>
+        <v>140</v>
       </c>
       <c r="S64" s="26"/>
       <c r="T64" s="26"/>
       <c r="U64" s="21" t="n">
         <f aca="false">SUM(H64:R64)</f>
-        <v>5</v>
+        <v>700</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="20" t="n">
-        <v>55</v>
-      </c>
-      <c r="B65" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C65" s="29"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="30" t="n">
-        <v>15</v>
-      </c>
-      <c r="G65" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="H65" s="26"/>
-      <c r="I65" s="26"/>
-      <c r="J65" s="26"/>
-      <c r="K65" s="26"/>
-      <c r="L65" s="26"/>
-      <c r="M65" s="26"/>
-      <c r="N65" s="30" t="n">
-        <v>3</v>
-      </c>
-      <c r="O65" s="30" t="n">
-        <v>3</v>
-      </c>
-      <c r="P65" s="30" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q65" s="30" t="n">
-        <v>3</v>
-      </c>
-      <c r="R65" s="30" t="n">
-        <v>3</v>
-      </c>
-      <c r="S65" s="26"/>
-      <c r="T65" s="26"/>
-      <c r="U65" s="21" t="n">
-        <f aca="false">SUM(H65:R65)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="20" t="n">
-        <v>56</v>
-      </c>
-      <c r="B66" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C66" s="29"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
-      <c r="F66" s="30" t="n">
-        <v>21</v>
-      </c>
-      <c r="G66" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="H66" s="26"/>
-      <c r="I66" s="26"/>
-      <c r="J66" s="26"/>
-      <c r="K66" s="26"/>
-      <c r="L66" s="26"/>
-      <c r="M66" s="26"/>
-      <c r="N66" s="30" t="n">
+      <c r="A65" s="20"/>
+      <c r="B65" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="33" t="n">
+        <f aca="false">SUM(F24,F64)</f>
+        <v>1120</v>
+      </c>
+      <c r="G65" s="33" t="n">
+        <f aca="false">SUM(G18:G23,G28:G63)</f>
+        <v>0</v>
+      </c>
+      <c r="H65" s="33" t="n">
+        <f aca="false">SUM(H18:H23,H28:H63)</f>
+        <v>140</v>
+      </c>
+      <c r="I65" s="33" t="n">
+        <f aca="false">SUM(I18:I23,I28:I63)</f>
+        <v>140</v>
+      </c>
+      <c r="J65" s="33" t="n">
+        <f aca="false">SUM(J18:J23,J28:J63)</f>
         <v>7</v>
       </c>
-      <c r="O66" s="30"/>
-      <c r="P66" s="30" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q66" s="30"/>
-      <c r="R66" s="30" t="n">
-        <v>7</v>
-      </c>
-      <c r="S66" s="26"/>
-      <c r="T66" s="26"/>
-      <c r="U66" s="21" t="n">
-        <f aca="false">SUM(H66:R66)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="20" t="n">
-        <v>57</v>
-      </c>
-      <c r="B67" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="30" t="n">
-        <v>12</v>
-      </c>
-      <c r="G67" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="H67" s="26"/>
-      <c r="I67" s="26"/>
-      <c r="J67" s="26"/>
-      <c r="K67" s="26"/>
-      <c r="L67" s="26"/>
-      <c r="M67" s="26"/>
-      <c r="N67" s="30" t="n">
-        <v>8</v>
-      </c>
-      <c r="O67" s="30" t="n">
-        <v>4</v>
-      </c>
-      <c r="P67" s="30"/>
-      <c r="Q67" s="30"/>
-      <c r="R67" s="30"/>
-      <c r="S67" s="26"/>
-      <c r="T67" s="26"/>
-      <c r="U67" s="21" t="n">
-        <f aca="false">SUM(H67:R67)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="20" t="n">
-        <v>58</v>
-      </c>
-      <c r="B68" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C68" s="29"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="30" t="n">
-        <f aca="false">(700-SUM(F26:F67))</f>
-        <v>55</v>
-      </c>
-      <c r="G68" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="H68" s="26"/>
-      <c r="I68" s="26"/>
-      <c r="J68" s="26"/>
-      <c r="K68" s="26"/>
-      <c r="L68" s="26"/>
-      <c r="M68" s="26"/>
-      <c r="N68" s="30" t="n">
-        <f aca="false">(140-SUM(N26:N67))</f>
-        <v>10</v>
-      </c>
-      <c r="O68" s="30" t="n">
-        <f aca="false">(140-SUM(O26:O67))</f>
-        <v>10</v>
-      </c>
-      <c r="P68" s="30" t="n">
-        <f aca="false">(140-SUM(P26:P67))</f>
-        <v>11</v>
-      </c>
-      <c r="Q68" s="30" t="n">
-        <f aca="false">(140-SUM(Q26:Q67))</f>
-        <v>12</v>
-      </c>
-      <c r="R68" s="30" t="n">
-        <f aca="false">(140-SUM(R26:R67))</f>
-        <v>12</v>
-      </c>
-      <c r="S68" s="26"/>
-      <c r="T68" s="26"/>
-      <c r="U68" s="21" t="n">
-        <f aca="false">SUM(H68:R68)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="20" t="n">
-        <v>59</v>
-      </c>
-      <c r="B69" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C69" s="29"/>
-      <c r="D69" s="29"/>
-      <c r="E69" s="29"/>
-      <c r="F69" s="30" t="n">
-        <f aca="false">SUM(F26:F68)</f>
-        <v>700</v>
-      </c>
-      <c r="G69" s="30"/>
-      <c r="H69" s="26"/>
-      <c r="I69" s="26"/>
-      <c r="J69" s="26"/>
-      <c r="K69" s="26"/>
-      <c r="L69" s="26"/>
-      <c r="M69" s="26"/>
-      <c r="N69" s="30" t="n">
-        <f aca="false">SUM(N26:N68)</f>
+      <c r="K65" s="33" t="n">
+        <f aca="false">SUM(K18:K23,K28:K63)</f>
+        <v>0</v>
+      </c>
+      <c r="L65" s="33" t="n">
+        <f aca="false">SUM(L18:L23,L28:L63)</f>
+        <v>0</v>
+      </c>
+      <c r="M65" s="33" t="n">
+        <f aca="false">SUM(M18:M23,M28:M63)</f>
+        <v>133</v>
+      </c>
+      <c r="N65" s="33" t="n">
+        <f aca="false">SUM(N18:N23,N28:N63)</f>
         <v>140</v>
       </c>
-      <c r="O69" s="30" t="n">
-        <f aca="false">SUM(O26:O68)</f>
+      <c r="O65" s="33" t="n">
+        <f aca="false">SUM(O18:O23,O28:O63)</f>
         <v>140</v>
       </c>
-      <c r="P69" s="30" t="n">
-        <f aca="false">SUM(P26:P68)</f>
+      <c r="P65" s="33" t="n">
+        <f aca="false">SUM(P18:P23,P28:P63)</f>
         <v>140</v>
       </c>
-      <c r="Q69" s="30" t="n">
-        <f aca="false">SUM(Q26:Q68)</f>
+      <c r="Q65" s="33" t="n">
+        <f aca="false">SUM(Q18:Q23,Q28:Q63)</f>
         <v>140</v>
       </c>
-      <c r="R69" s="30" t="n">
-        <f aca="false">SUM(R26:R68)</f>
+      <c r="R65" s="33" t="n">
+        <f aca="false">SUM(R18:R23,R28:R63)</f>
         <v>140</v>
       </c>
-      <c r="S69" s="26"/>
-      <c r="T69" s="26"/>
-      <c r="U69" s="21" t="n">
-        <f aca="false">SUM(H69:R69)</f>
-        <v>700</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="20"/>
-      <c r="B70" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="33" t="n">
-        <f aca="false">SUM(F23,F69)</f>
-        <v>1120</v>
-      </c>
-      <c r="G70" s="33" t="n">
-        <f aca="false">SUM(G13:G22,G26:G68)</f>
-        <v>0</v>
-      </c>
-      <c r="H70" s="33" t="n">
-        <f aca="false">SUM(H13:H22,H26:H68)</f>
-        <v>140</v>
-      </c>
-      <c r="I70" s="33" t="n">
-        <f aca="false">SUM(I13:I22,I26:I68)</f>
-        <v>140</v>
-      </c>
-      <c r="J70" s="33" t="n">
-        <f aca="false">SUM(J13:J22,J26:J68)</f>
-        <v>7</v>
-      </c>
-      <c r="K70" s="33" t="n">
-        <f aca="false">SUM(K13:K22,K26:K68)</f>
-        <v>0</v>
-      </c>
-      <c r="L70" s="33" t="n">
-        <f aca="false">SUM(L13:L22,L26:L68)</f>
-        <v>0</v>
-      </c>
-      <c r="M70" s="33" t="n">
-        <f aca="false">SUM(M13:M22,M26:M68)</f>
-        <v>133</v>
-      </c>
-      <c r="N70" s="33" t="n">
-        <f aca="false">SUM(N13:N22,N26:N68)</f>
-        <v>140</v>
-      </c>
-      <c r="O70" s="33" t="n">
-        <f aca="false">SUM(O13:O22,O26:O68)</f>
-        <v>140</v>
-      </c>
-      <c r="P70" s="33" t="n">
-        <f aca="false">SUM(P13:P22,P26:P68)</f>
-        <v>140</v>
-      </c>
-      <c r="Q70" s="33" t="n">
-        <f aca="false">SUM(Q13:Q22,Q26:Q68)</f>
-        <v>140</v>
-      </c>
-      <c r="R70" s="33" t="n">
-        <f aca="false">SUM(R13:R22,R26:R68)</f>
-        <v>140</v>
-      </c>
-      <c r="S70" s="33" t="n">
-        <f aca="false">SUM(S13:S22,S26:S68)</f>
-        <v>0</v>
-      </c>
-      <c r="T70" s="33" t="n">
-        <f aca="false">SUM(T13:T22,T26:T68)</f>
-        <v>0</v>
-      </c>
-      <c r="U70" s="33" t="n">
-        <f aca="false">SUM(U13:U22,U26:U68)</f>
-        <v>1120</v>
-      </c>
-    </row>
+      <c r="S65" s="33" t="n">
+        <f aca="false">SUM(S18:S23,S28:S63)</f>
+        <v>0</v>
+      </c>
+      <c r="T65" s="33" t="n">
+        <f aca="false">SUM(T18:T23,T28:T63)</f>
+        <v>0</v>
+      </c>
+      <c r="U65" s="33" t="n">
+        <f aca="false">SUM(U18:U23,U28:U63)</f>
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="81">
+  <mergeCells count="76">
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:U2"/>
@@ -3835,9 +3535,9 @@
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B22:E22"/>
     <mergeCell ref="B23:E23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="H24:U24"/>
-    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="H25:U25"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B28:E28"/>
@@ -3878,19 +3578,18 @@
     <mergeCell ref="B63:E63"/>
     <mergeCell ref="B64:E64"/>
     <mergeCell ref="B65:E65"/>
-    <mergeCell ref="B66:E66"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="B70:E70"/>
   </mergeCells>
-  <conditionalFormatting sqref="V26:V68">
-    <cfRule type="containsText" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="0"/>
-    <cfRule type="containsText" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="1"/>
+  <conditionalFormatting sqref="V58:V63 V28:V29 V31 V33:V36 V38:V41 V43 V45:V46 V48:V50 V52 V54:V56">
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("FALSE",V28)))</formula>
+    </cfRule>
+    <cfRule type="containsText" priority="3" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="1">
+      <formula>NOT(ISERROR(SEARCH("TRUE",V28)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.984027777777778" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3905,25 +3604,25 @@
   </sheetPr>
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.14285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1428571428571"/>
-    <col collapsed="false" hidden="true" max="3" min="3" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.1428571428571"/>
-    <col collapsed="false" hidden="true" max="5" min="5" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="29" min="6" style="0" width="3.41836734693878"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="4.13775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="0" width="8.70918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.14"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="6" style="0" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="4.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4006,7 +3705,7 @@
       <c r="F3" s="39"/>
       <c r="G3" s="39"/>
       <c r="H3" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -4033,7 +3732,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B4" s="41"/>
       <c r="C4" s="42"/>
@@ -4045,7 +3744,7 @@
       <c r="F4" s="43"/>
       <c r="G4" s="43"/>
       <c r="H4" s="41" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I4" s="41"/>
       <c r="J4" s="41"/>
@@ -4072,7 +3771,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="45" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B5" s="45"/>
       <c r="C5" s="46"/>
@@ -4109,7 +3808,7 @@
     </row>
     <row r="6" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="49" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B6" s="49"/>
       <c r="C6" s="49"/>
@@ -4117,7 +3816,7 @@
       <c r="E6" s="49"/>
       <c r="F6" s="49"/>
       <c r="G6" s="50" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H6" s="50"/>
       <c r="I6" s="50"/>
@@ -4146,7 +3845,7 @@
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="51"/>
       <c r="B7" s="52" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C7" s="52"/>
       <c r="D7" s="52"/>
@@ -4245,7 +3944,7 @@
         <v>#REF!</v>
       </c>
       <c r="AD7" s="54" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5161,7 +4860,7 @@
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="71" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C34" s="71"/>
       <c r="D34" s="71"/>
@@ -5313,7 +5012,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.709722222222222" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
tidplan version 0.2 should be finished
</commit_message>
<xml_diff>
--- a/doc/projektplan/05Tidplan01.xlsx
+++ b/doc/projektplan/05Tidplan01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lil_b\Documents\tsea29-taxi\doc\projektplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900CF8E6-C305-402A-A106-205326237D75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA19F702-3C7E-40B4-96DB-7F39AAC84287}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="138">
   <si>
     <t xml:space="preserve">Godkännande av </t>
   </si>
@@ -55,9 +55,6 @@
     <t>Version: 0.2</t>
   </si>
   <si>
-    <t>NH, EH, YH</t>
-  </si>
-  <si>
     <t>Kurs: TSEA29</t>
   </si>
   <si>
@@ -392,6 +389,63 @@
   </si>
   <si>
     <t xml:space="preserve">Summa antal timmar:  </t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>EH</t>
+  </si>
+  <si>
+    <t>JC</t>
+  </si>
+  <si>
+    <t>DD,JB</t>
+  </si>
+  <si>
+    <t>YH, JA</t>
+  </si>
+  <si>
+    <t>NH,EH</t>
+  </si>
+  <si>
+    <t>NH, Alla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YH </t>
+  </si>
+  <si>
+    <t>JC,YH</t>
+  </si>
+  <si>
+    <t>DD, EH, Alla</t>
+  </si>
+  <si>
+    <t>JA,YH</t>
+  </si>
+  <si>
+    <t>JB, EH</t>
+  </si>
+  <si>
+    <t>JB, JC</t>
+  </si>
+  <si>
+    <t>JA, JC, DD</t>
+  </si>
+  <si>
+    <t>EH, NH, JB, YH</t>
+  </si>
+  <si>
+    <t>YH, DD</t>
+  </si>
+  <si>
+    <t>EH, JB</t>
+  </si>
+  <si>
+    <t>NH, DD</t>
+  </si>
+  <si>
+    <t>EH, JA</t>
   </si>
 </sst>
 </file>
@@ -1506,8 +1560,8 @@
   </sheetPr>
   <dimension ref="A1:U86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1518,7 +1572,7 @@
     <col min="4" max="4" width="47.42578125" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" customWidth="1"/>
     <col min="6" max="6" width="7.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="20" width="4.42578125" customWidth="1"/>
     <col min="21" max="21" width="5.85546875" customWidth="1"/>
     <col min="22" max="1014" width="8.7109375" customWidth="1"/>
@@ -1627,7 +1681,7 @@
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="6" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
@@ -1637,7 +1691,7 @@
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="18"/>
@@ -1645,7 +1699,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -1664,20 +1718,20 @@
     </row>
     <row r="6" spans="1:21" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="H6" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -1695,19 +1749,19 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="21" t="s">
         <v>16</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>17</v>
       </c>
       <c r="H7" s="22">
         <v>40</v>
@@ -1753,7 +1807,7 @@
     <row r="8" spans="1:21" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1762,7 +1816,7 @@
         <v>1120</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="25">
         <v>40</v>
@@ -1801,7 +1855,7 @@
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="22"/>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1810,7 +1864,7 @@
         <v>220</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="25">
         <v>40</v>
@@ -1839,7 +1893,7 @@
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1848,7 +1902,7 @@
         <v>900</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
@@ -1880,20 +1934,20 @@
     </row>
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="H11" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -1911,19 +1965,19 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="21" t="s">
         <v>16</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>17</v>
       </c>
       <c r="H12" s="22">
         <v>40</v>
@@ -1969,42 +2023,19 @@
     <row r="13" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="56"/>
       <c r="E13" s="56"/>
-      <c r="F13" s="31">
-        <f>SUM(F14:F16)</f>
-        <v>100</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="21">
-        <f t="shared" ref="H13:M13" si="0">SUM(H14:H16)</f>
-        <v>30</v>
-      </c>
-      <c r="I13" s="21">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="J13" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
       <c r="N13" s="28"/>
       <c r="O13" s="28"/>
       <c r="P13" s="28"/>
@@ -2012,17 +2043,14 @@
       <c r="R13" s="28"/>
       <c r="S13" s="28"/>
       <c r="T13" s="28"/>
-      <c r="U13" s="21">
-        <f>SUM(U14:U16)</f>
-        <v>100</v>
-      </c>
+      <c r="U13" s="21"/>
     </row>
     <row r="14" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2031,7 +2059,7 @@
         <v>20</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="25">
         <v>10</v>
@@ -2060,7 +2088,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2069,7 +2097,7 @@
         <v>40</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15" s="25">
         <v>20</v>
@@ -2098,7 +2126,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2107,7 +2135,7 @@
         <v>40</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H16" s="25"/>
       <c r="I16" s="25">
@@ -2134,7 +2162,7 @@
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="22"/>
       <c r="B17" s="56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="56"/>
@@ -2161,7 +2189,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2170,7 +2198,7 @@
         <v>40</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" s="25"/>
       <c r="I18" s="25"/>
@@ -2197,7 +2225,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2206,7 +2234,7 @@
         <v>20</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>19</v>
+        <v>123</v>
       </c>
       <c r="H19" s="25"/>
       <c r="I19" s="25">
@@ -2235,7 +2263,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2244,7 +2272,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="25" t="s">
-        <v>19</v>
+        <v>130</v>
       </c>
       <c r="H20" s="25"/>
       <c r="I20" s="25">
@@ -2271,7 +2299,7 @@
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="22"/>
       <c r="B21" s="56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="56"/>
       <c r="D21" s="56"/>
@@ -2298,7 +2326,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2307,7 +2335,7 @@
         <v>21</v>
       </c>
       <c r="G22" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="25">
         <v>7</v>
@@ -2336,7 +2364,7 @@
     <row r="23" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2345,9 +2373,7 @@
         <f>(220-SUM(F14:F22))</f>
         <v>19</v>
       </c>
-      <c r="G23" s="25" t="s">
-        <v>19</v>
-      </c>
+      <c r="G23" s="25"/>
       <c r="H23" s="25">
         <f>(H8-SUM(H14:H22))</f>
         <v>3</v>
@@ -2378,7 +2404,7 @@
     <row r="24" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2387,9 +2413,7 @@
         <f>SUM(F14:F23)</f>
         <v>220</v>
       </c>
-      <c r="G24" s="25" t="s">
-        <v>19</v>
-      </c>
+      <c r="G24" s="25"/>
       <c r="H24" s="25">
         <f>SUM(H14:H23)</f>
         <v>40</v>
@@ -2419,20 +2443,20 @@
     </row>
     <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="H25" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
@@ -2450,19 +2474,19 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="21" t="s">
         <v>16</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>17</v>
       </c>
       <c r="H26" s="22">
         <v>40</v>
@@ -2508,7 +2532,7 @@
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
       <c r="B27" s="56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="56"/>
       <c r="D27" s="56"/>
@@ -2535,7 +2559,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2544,7 +2568,7 @@
         <v>55</v>
       </c>
       <c r="G28" s="25" t="s">
-        <v>19</v>
+        <v>128</v>
       </c>
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
@@ -2573,7 +2597,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2582,7 +2606,7 @@
         <v>60</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
@@ -2609,7 +2633,7 @@
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="22"/>
       <c r="B30" s="56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="56"/>
       <c r="D30" s="56"/>
@@ -2636,7 +2660,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="57"/>
       <c r="D31" s="57"/>
@@ -2645,7 +2669,7 @@
         <v>40</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
@@ -2672,7 +2696,7 @@
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="22"/>
       <c r="B32" s="56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="56"/>
       <c r="D32" s="56"/>
@@ -2699,7 +2723,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="57"/>
       <c r="D33" s="57"/>
@@ -2708,7 +2732,7 @@
         <v>35</v>
       </c>
       <c r="G33" s="25" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
@@ -2735,7 +2759,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="57"/>
       <c r="D34" s="57"/>
@@ -2744,7 +2768,7 @@
         <v>35</v>
       </c>
       <c r="G34" s="25" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
@@ -2771,7 +2795,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C35" s="57"/>
       <c r="D35" s="57"/>
@@ -2780,7 +2804,7 @@
         <v>20</v>
       </c>
       <c r="G35" s="25" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="H35" s="28"/>
       <c r="I35" s="28"/>
@@ -2807,7 +2831,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C36" s="57"/>
       <c r="D36" s="57"/>
@@ -2816,7 +2840,7 @@
         <v>30</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="H36" s="28"/>
       <c r="I36" s="28"/>
@@ -2841,7 +2865,7 @@
     <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="22"/>
       <c r="B37" s="56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" s="56"/>
       <c r="D37" s="56"/>
@@ -2868,7 +2892,7 @@
         <v>15</v>
       </c>
       <c r="B38" s="57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" s="57"/>
       <c r="D38" s="57"/>
@@ -2877,7 +2901,7 @@
         <v>30</v>
       </c>
       <c r="G38" s="25" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="H38" s="28"/>
       <c r="I38" s="28"/>
@@ -2904,7 +2928,7 @@
         <v>16</v>
       </c>
       <c r="B39" s="57" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="57"/>
       <c r="D39" s="57"/>
@@ -2913,7 +2937,7 @@
         <v>20</v>
       </c>
       <c r="G39" s="25" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="H39" s="28"/>
       <c r="I39" s="28"/>
@@ -2940,7 +2964,7 @@
         <v>17</v>
       </c>
       <c r="B40" s="57" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" s="57"/>
       <c r="D40" s="57"/>
@@ -2949,7 +2973,7 @@
         <v>30</v>
       </c>
       <c r="G40" s="25" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="H40" s="28"/>
       <c r="I40" s="28"/>
@@ -2978,7 +3002,7 @@
         <v>18</v>
       </c>
       <c r="B41" s="57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="57"/>
       <c r="D41" s="57"/>
@@ -2987,7 +3011,7 @@
         <v>40</v>
       </c>
       <c r="G41" s="25" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="H41" s="28"/>
       <c r="I41" s="28"/>
@@ -3014,7 +3038,7 @@
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="22"/>
       <c r="B42" s="56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C42" s="56"/>
       <c r="D42" s="56"/>
@@ -3041,7 +3065,7 @@
         <v>19</v>
       </c>
       <c r="B43" s="57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43" s="57"/>
       <c r="D43" s="57"/>
@@ -3050,7 +3074,7 @@
         <v>40</v>
       </c>
       <c r="G43" s="25" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
@@ -3075,7 +3099,7 @@
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="22"/>
       <c r="B44" s="56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" s="56"/>
       <c r="D44" s="56"/>
@@ -3102,7 +3126,7 @@
         <v>20</v>
       </c>
       <c r="B45" s="57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C45" s="57"/>
       <c r="D45" s="57"/>
@@ -3111,7 +3135,7 @@
         <v>40</v>
       </c>
       <c r="G45" s="25" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="H45" s="28"/>
       <c r="I45" s="28"/>
@@ -3140,7 +3164,7 @@
         <v>21</v>
       </c>
       <c r="B46" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46" s="57"/>
       <c r="D46" s="57"/>
@@ -3149,7 +3173,7 @@
         <v>20</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="H46" s="28"/>
       <c r="I46" s="28"/>
@@ -3176,7 +3200,7 @@
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" s="22"/>
       <c r="B47" s="56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C47" s="56"/>
       <c r="D47" s="56"/>
@@ -3203,7 +3227,7 @@
         <v>22</v>
       </c>
       <c r="B48" s="57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C48" s="57"/>
       <c r="D48" s="57"/>
@@ -3212,7 +3236,7 @@
         <v>15</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="H48" s="28"/>
       <c r="I48" s="28"/>
@@ -3239,7 +3263,7 @@
         <v>23</v>
       </c>
       <c r="B49" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C49" s="57"/>
       <c r="D49" s="57"/>
@@ -3248,7 +3272,7 @@
         <v>30</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
@@ -3277,7 +3301,7 @@
         <v>24</v>
       </c>
       <c r="B50" s="57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C50" s="57"/>
       <c r="D50" s="57"/>
@@ -3286,7 +3310,7 @@
         <v>30</v>
       </c>
       <c r="G50" s="25" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="H50" s="28"/>
       <c r="I50" s="28"/>
@@ -3313,7 +3337,7 @@
     <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" s="22"/>
       <c r="B51" s="56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C51" s="56"/>
       <c r="D51" s="56"/>
@@ -3340,7 +3364,7 @@
         <v>25</v>
       </c>
       <c r="B52" s="57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C52" s="57"/>
       <c r="D52" s="57"/>
@@ -3349,7 +3373,7 @@
         <v>20</v>
       </c>
       <c r="G52" s="25" t="s">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="H52" s="28"/>
       <c r="I52" s="28"/>
@@ -3374,7 +3398,7 @@
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" s="22"/>
       <c r="B53" s="56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C53" s="56"/>
       <c r="D53" s="56"/>
@@ -3401,7 +3425,7 @@
         <v>26</v>
       </c>
       <c r="B54" s="57" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" s="57"/>
       <c r="D54" s="57"/>
@@ -3410,7 +3434,7 @@
         <v>10</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="H54" s="28"/>
       <c r="I54" s="28"/>
@@ -3437,7 +3461,7 @@
         <v>27</v>
       </c>
       <c r="B55" s="57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" s="57"/>
       <c r="D55" s="57"/>
@@ -3446,7 +3470,7 @@
         <v>30</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>19</v>
+        <v>134</v>
       </c>
       <c r="H55" s="28"/>
       <c r="I55" s="28"/>
@@ -3471,7 +3495,7 @@
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" s="22"/>
       <c r="B56" s="56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C56" s="56"/>
       <c r="D56" s="56"/>
@@ -3498,7 +3522,7 @@
         <v>28</v>
       </c>
       <c r="B57" s="57" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C57" s="57"/>
       <c r="D57" s="57"/>
@@ -3507,7 +3531,7 @@
         <v>70</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H57" s="28"/>
       <c r="I57" s="28"/>
@@ -3534,7 +3558,7 @@
         <v>29</v>
       </c>
       <c r="B58" s="57" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" s="57"/>
       <c r="D58" s="57"/>
@@ -3543,7 +3567,7 @@
         <v>20</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>19</v>
+        <v>132</v>
       </c>
       <c r="H58" s="28"/>
       <c r="I58" s="28"/>
@@ -3572,7 +3596,7 @@
         <v>30</v>
       </c>
       <c r="B59" s="57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" s="57"/>
       <c r="D59" s="57"/>
@@ -3581,7 +3605,7 @@
         <v>20</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="H59" s="28"/>
       <c r="I59" s="28"/>
@@ -3610,7 +3634,7 @@
         <v>33</v>
       </c>
       <c r="B60" s="57" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C60" s="57"/>
       <c r="D60" s="57"/>
@@ -3619,7 +3643,7 @@
         <v>20</v>
       </c>
       <c r="G60" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H60" s="28"/>
       <c r="I60" s="28"/>
@@ -3652,7 +3676,7 @@
     <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" s="22"/>
       <c r="B61" s="56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C61" s="56"/>
       <c r="D61" s="56"/>
@@ -3679,7 +3703,7 @@
         <v>32</v>
       </c>
       <c r="B62" s="57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C62" s="57"/>
       <c r="D62" s="57"/>
@@ -3688,7 +3712,7 @@
         <v>35</v>
       </c>
       <c r="G62" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H62" s="28"/>
       <c r="I62" s="28"/>
@@ -3721,7 +3745,7 @@
     <row r="63" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A63" s="22"/>
       <c r="B63" s="58" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C63" s="58"/>
       <c r="D63" s="58"/>
@@ -3730,9 +3754,7 @@
         <f>(900-SUM(F28:F62))</f>
         <v>105</v>
       </c>
-      <c r="G63" s="32" t="s">
-        <v>19</v>
-      </c>
+      <c r="G63" s="32"/>
       <c r="H63" s="28"/>
       <c r="I63" s="28"/>
       <c r="J63" s="28"/>
@@ -3769,7 +3791,7 @@
     <row r="64" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A64" s="22"/>
       <c r="B64" s="57" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C64" s="57"/>
       <c r="D64" s="57"/>
@@ -3815,7 +3837,7 @@
     <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="22"/>
       <c r="B65" s="59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C65" s="59"/>
       <c r="D65" s="59"/>
@@ -3860,7 +3882,7 @@
     </row>
     <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -3869,7 +3891,7 @@
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
@@ -3890,7 +3912,7 @@
         <v>1</v>
       </c>
       <c r="B67" s="60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C67" s="60"/>
       <c r="D67" s="60"/>
@@ -3898,7 +3920,7 @@
       <c r="F67" s="60"/>
       <c r="G67" s="60"/>
       <c r="H67" s="61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I67" s="61"/>
       <c r="J67" s="61"/>
@@ -3919,7 +3941,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C68" s="60"/>
       <c r="D68" s="60"/>
@@ -3927,7 +3949,7 @@
       <c r="F68" s="60"/>
       <c r="G68" s="60"/>
       <c r="H68" s="61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I68" s="61"/>
       <c r="J68" s="61"/>
@@ -3948,7 +3970,7 @@
         <v>3</v>
       </c>
       <c r="B69" s="60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C69" s="60"/>
       <c r="D69" s="60"/>
@@ -3956,7 +3978,7 @@
       <c r="F69" s="60"/>
       <c r="G69" s="60"/>
       <c r="H69" s="61" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I69" s="61"/>
       <c r="J69" s="61"/>
@@ -3977,7 +3999,7 @@
         <v>4</v>
       </c>
       <c r="B70" s="60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C70" s="60"/>
       <c r="D70" s="60"/>
@@ -3985,7 +4007,7 @@
       <c r="F70" s="60"/>
       <c r="G70" s="60"/>
       <c r="H70" s="61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I70" s="61"/>
       <c r="J70" s="61"/>
@@ -4006,7 +4028,7 @@
         <v>5</v>
       </c>
       <c r="B71" s="60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C71" s="60"/>
       <c r="D71" s="60"/>
@@ -4014,7 +4036,7 @@
       <c r="F71" s="60"/>
       <c r="G71" s="60"/>
       <c r="H71" s="61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I71" s="61"/>
       <c r="J71" s="61"/>
@@ -4035,7 +4057,7 @@
         <v>6</v>
       </c>
       <c r="B72" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C72" s="60"/>
       <c r="D72" s="60"/>
@@ -4043,7 +4065,7 @@
       <c r="F72" s="60"/>
       <c r="G72" s="60"/>
       <c r="H72" s="61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I72" s="61"/>
       <c r="J72" s="61"/>
@@ -4064,7 +4086,7 @@
         <v>7</v>
       </c>
       <c r="B73" s="60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C73" s="60"/>
       <c r="D73" s="60"/>
@@ -4072,7 +4094,7 @@
       <c r="F73" s="60"/>
       <c r="G73" s="60"/>
       <c r="H73" s="61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I73" s="61"/>
       <c r="J73" s="61"/>
@@ -4093,7 +4115,7 @@
         <v>8</v>
       </c>
       <c r="B74" s="60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C74" s="60"/>
       <c r="D74" s="60"/>
@@ -4101,7 +4123,7 @@
       <c r="F74" s="60"/>
       <c r="G74" s="60"/>
       <c r="H74" s="61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I74" s="61"/>
       <c r="J74" s="61"/>
@@ -4122,7 +4144,7 @@
         <v>9</v>
       </c>
       <c r="B75" s="60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C75" s="60"/>
       <c r="D75" s="60"/>
@@ -4130,7 +4152,7 @@
       <c r="F75" s="60"/>
       <c r="G75" s="60"/>
       <c r="H75" s="61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I75" s="61"/>
       <c r="J75" s="61"/>
@@ -4151,7 +4173,7 @@
         <v>10</v>
       </c>
       <c r="B76" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C76" s="60"/>
       <c r="D76" s="60"/>
@@ -4159,7 +4181,7 @@
       <c r="F76" s="60"/>
       <c r="G76" s="60"/>
       <c r="H76" s="61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I76" s="61"/>
       <c r="J76" s="61"/>
@@ -4180,7 +4202,7 @@
         <v>11</v>
       </c>
       <c r="B77" s="60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C77" s="60"/>
       <c r="D77" s="60"/>
@@ -4188,7 +4210,7 @@
       <c r="F77" s="60"/>
       <c r="G77" s="60"/>
       <c r="H77" s="61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I77" s="61"/>
       <c r="J77" s="61"/>
@@ -4209,7 +4231,7 @@
         <v>12</v>
       </c>
       <c r="B78" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C78" s="60"/>
       <c r="D78" s="60"/>
@@ -4217,7 +4239,7 @@
       <c r="F78" s="60"/>
       <c r="G78" s="60"/>
       <c r="H78" s="61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I78" s="61"/>
       <c r="J78" s="61"/>
@@ -4235,20 +4257,20 @@
     </row>
     <row r="79" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G79" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G79" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="H79" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
@@ -4269,7 +4291,7 @@
         <v>0</v>
       </c>
       <c r="B80" s="60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C80" s="60"/>
       <c r="D80" s="60"/>
@@ -4277,7 +4299,7 @@
       <c r="F80" s="60"/>
       <c r="G80" s="60"/>
       <c r="H80" s="61" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I80" s="61"/>
       <c r="J80" s="61"/>
@@ -4298,7 +4320,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C81" s="60"/>
       <c r="D81" s="60"/>
@@ -4306,7 +4328,7 @@
       <c r="F81" s="60"/>
       <c r="G81" s="60"/>
       <c r="H81" s="61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I81" s="61"/>
       <c r="J81" s="61"/>
@@ -4327,7 +4349,7 @@
         <v>2</v>
       </c>
       <c r="B82" s="60" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82" s="60"/>
       <c r="D82" s="60"/>
@@ -4335,7 +4357,7 @@
       <c r="F82" s="60"/>
       <c r="G82" s="60"/>
       <c r="H82" s="61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I82" s="61"/>
       <c r="J82" s="61"/>
@@ -4356,7 +4378,7 @@
         <v>3</v>
       </c>
       <c r="B83" s="60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C83" s="60"/>
       <c r="D83" s="60"/>
@@ -4364,7 +4386,7 @@
       <c r="F83" s="60"/>
       <c r="G83" s="60"/>
       <c r="H83" s="61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I83" s="61"/>
       <c r="J83" s="61"/>
@@ -4385,7 +4407,7 @@
         <v>4</v>
       </c>
       <c r="B84" s="62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C84" s="62"/>
       <c r="D84" s="62"/>
@@ -4393,7 +4415,7 @@
       <c r="F84" s="62"/>
       <c r="G84" s="62"/>
       <c r="H84" s="61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I84" s="61"/>
       <c r="J84" s="61"/>
@@ -4414,7 +4436,7 @@
         <v>5</v>
       </c>
       <c r="B85" s="60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C85" s="60"/>
       <c r="D85" s="60"/>
@@ -4422,7 +4444,7 @@
       <c r="F85" s="60"/>
       <c r="G85" s="60"/>
       <c r="H85" s="61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I85" s="61"/>
       <c r="J85" s="61"/>
@@ -4443,7 +4465,7 @@
         <v>6</v>
       </c>
       <c r="B86" s="60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C86" s="60"/>
       <c r="D86" s="60"/>
@@ -4451,7 +4473,7 @@
       <c r="F86" s="60"/>
       <c r="G86" s="60"/>
       <c r="H86" s="61" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I86" s="61"/>
       <c r="J86" s="61"/>
@@ -4626,7 +4648,7 @@
   <sheetData>
     <row r="1" spans="1:30" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="63"/>
       <c r="C1" s="63"/>
@@ -4709,7 +4731,7 @@
       <c r="F3" s="67"/>
       <c r="G3" s="67"/>
       <c r="H3" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -4736,7 +4758,7 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="69"/>
       <c r="C4" s="36"/>
@@ -4748,7 +4770,7 @@
       <c r="F4" s="70"/>
       <c r="G4" s="70"/>
       <c r="H4" s="69" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I4" s="69"/>
       <c r="J4" s="69"/>
@@ -4775,7 +4797,7 @@
     </row>
     <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="72"/>
       <c r="C5" s="37"/>
@@ -4812,7 +4834,7 @@
     </row>
     <row r="6" spans="1:30" s="20" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="75" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="75"/>
       <c r="C6" s="75"/>
@@ -4820,7 +4842,7 @@
       <c r="E6" s="75"/>
       <c r="F6" s="75"/>
       <c r="G6" s="76" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H6" s="76"/>
       <c r="I6" s="76"/>
@@ -4849,7 +4871,7 @@
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" s="38"/>
       <c r="B7" s="77" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" s="77"/>
       <c r="D7" s="77"/>
@@ -4948,7 +4970,7 @@
         <v>#REF!</v>
       </c>
       <c r="AD7" s="40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
@@ -5864,7 +5886,7 @@
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
       <c r="B34" s="81" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C34" s="81"/>
       <c r="D34" s="81"/>

</xml_diff>

<commit_message>
report time for JC, NH, EH & YH
</commit_message>
<xml_diff>
--- a/doc/projektplan/05Tidplan01.xlsx
+++ b/doc/projektplan/05Tidplan01.xlsx
@@ -5,12 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Basplan" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Summering TID" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Basplan" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="115">
   <si>
     <t xml:space="preserve">Godkännande av </t>
   </si>
@@ -367,47 +365,16 @@
   </si>
   <si>
     <t xml:space="preserve">Godkännande av leverans, upplösning av projektgrupp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUMMERING AV TID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datum:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beställare:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utfärdare:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kurs:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESURS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEDLAGD TID (per vecka)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Namn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summa antal timmar:  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -498,20 +465,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -551,7 +504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="11">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -629,118 +582,6 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -767,7 +608,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -888,10 +729,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -946,170 +783,6 @@
     </xf>
     <xf numFmtId="164" fontId="13" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1217,32 +890,6 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.71"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:U89"/>
@@ -1254,10 +901,10 @@
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.13"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="47.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="8" style="0" width="5.55"/>
@@ -2277,7 +1924,7 @@
       <c r="P28" s="23"/>
       <c r="Q28" s="23"/>
       <c r="R28" s="23"/>
-      <c r="S28" s="30"/>
+      <c r="S28" s="25"/>
       <c r="T28" s="26"/>
       <c r="U28" s="21" t="n">
         <f aca="false">SUM(H28:S28)</f>
@@ -2315,7 +1962,7 @@
       <c r="P29" s="23"/>
       <c r="Q29" s="23"/>
       <c r="R29" s="23"/>
-      <c r="S29" s="30"/>
+      <c r="S29" s="25"/>
       <c r="T29" s="26"/>
       <c r="U29" s="21" t="n">
         <f aca="false">SUM(H29:S29)</f>
@@ -2351,13 +1998,13 @@
       <c r="A31" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="32" t="n">
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="31" t="n">
         <v>40</v>
       </c>
       <c r="G31" s="23" t="s">
@@ -2369,16 +2016,16 @@
       <c r="K31" s="26"/>
       <c r="L31" s="26"/>
       <c r="M31" s="26"/>
-      <c r="N31" s="32" t="n">
+      <c r="N31" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="O31" s="32" t="n">
+      <c r="O31" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="P31" s="32"/>
-      <c r="Q31" s="32"/>
-      <c r="R31" s="32"/>
-      <c r="S31" s="30"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="31"/>
+      <c r="S31" s="25"/>
       <c r="T31" s="26"/>
       <c r="U31" s="21" t="n">
         <f aca="false">SUM(H31:S31)</f>
@@ -2414,13 +2061,13 @@
       <c r="A33" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="32" t="n">
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="31" t="n">
         <v>25</v>
       </c>
       <c r="G33" s="23" t="s">
@@ -2432,14 +2079,14 @@
       <c r="K33" s="26"/>
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="32" t="n">
+      <c r="N33" s="31"/>
+      <c r="O33" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="32"/>
-      <c r="R33" s="32"/>
-      <c r="S33" s="30"/>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="31"/>
+      <c r="R33" s="31"/>
+      <c r="S33" s="25"/>
       <c r="T33" s="26"/>
       <c r="U33" s="21" t="n">
         <f aca="false">SUM(H33:S33)</f>
@@ -2450,13 +2097,13 @@
       <c r="A34" s="20" t="n">
         <v>12</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32" t="n">
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="31" t="n">
         <v>25</v>
       </c>
       <c r="G34" s="23" t="s">
@@ -2468,16 +2115,16 @@
       <c r="K34" s="26"/>
       <c r="L34" s="26"/>
       <c r="M34" s="26"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32" t="n">
+      <c r="N34" s="31"/>
+      <c r="O34" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="P34" s="32" t="n">
+      <c r="P34" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="Q34" s="32"/>
-      <c r="R34" s="32"/>
-      <c r="S34" s="30"/>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="31"/>
+      <c r="S34" s="25"/>
       <c r="T34" s="26"/>
       <c r="U34" s="21" t="n">
         <f aca="false">SUM(H34:S34)</f>
@@ -2488,13 +2135,13 @@
       <c r="A35" s="20" t="n">
         <v>13</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="32" t="n">
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="31" t="n">
         <v>20</v>
       </c>
       <c r="G35" s="23" t="s">
@@ -2506,14 +2153,14 @@
       <c r="K35" s="26"/>
       <c r="L35" s="26"/>
       <c r="M35" s="26"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="32" t="n">
+      <c r="N35" s="31"/>
+      <c r="O35" s="31"/>
+      <c r="P35" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="Q35" s="32"/>
-      <c r="R35" s="32"/>
-      <c r="S35" s="30"/>
+      <c r="Q35" s="31"/>
+      <c r="R35" s="31"/>
+      <c r="S35" s="25"/>
       <c r="T35" s="26"/>
       <c r="U35" s="21" t="n">
         <f aca="false">SUM(H35:S35)</f>
@@ -2524,13 +2171,13 @@
       <c r="A36" s="20" t="n">
         <v>14</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32" t="n">
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="31" t="n">
         <v>20</v>
       </c>
       <c r="G36" s="23" t="s">
@@ -2542,14 +2189,14 @@
       <c r="K36" s="26"/>
       <c r="L36" s="26"/>
       <c r="M36" s="26"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32" t="n">
+      <c r="N36" s="31"/>
+      <c r="O36" s="31"/>
+      <c r="P36" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="Q36" s="32"/>
-      <c r="R36" s="32"/>
-      <c r="S36" s="30"/>
+      <c r="Q36" s="31"/>
+      <c r="R36" s="31"/>
+      <c r="S36" s="25"/>
       <c r="T36" s="26"/>
       <c r="U36" s="21" t="n">
         <f aca="false">SUM(H36:S36)</f>
@@ -2585,13 +2232,13 @@
       <c r="A38" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="32" t="n">
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="31" t="n">
         <v>30</v>
       </c>
       <c r="G38" s="23" t="s">
@@ -2603,14 +2250,14 @@
       <c r="K38" s="26"/>
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="32" t="n">
+      <c r="N38" s="31"/>
+      <c r="O38" s="31"/>
+      <c r="P38" s="31"/>
+      <c r="Q38" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="R38" s="32"/>
-      <c r="S38" s="30"/>
+      <c r="R38" s="31"/>
+      <c r="S38" s="25"/>
       <c r="T38" s="26"/>
       <c r="U38" s="21" t="n">
         <f aca="false">SUM(H38:S38)</f>
@@ -2621,13 +2268,13 @@
       <c r="A39" s="20" t="n">
         <v>16</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="32" t="n">
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="31" t="n">
         <v>20</v>
       </c>
       <c r="G39" s="23" t="s">
@@ -2639,14 +2286,14 @@
       <c r="K39" s="26"/>
       <c r="L39" s="26"/>
       <c r="M39" s="26"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="32" t="n">
+      <c r="N39" s="31"/>
+      <c r="O39" s="31"/>
+      <c r="P39" s="31"/>
+      <c r="Q39" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="R39" s="32"/>
-      <c r="S39" s="30"/>
+      <c r="R39" s="31"/>
+      <c r="S39" s="25"/>
       <c r="T39" s="26"/>
       <c r="U39" s="21" t="n">
         <f aca="false">SUM(H39:S39)</f>
@@ -2657,13 +2304,13 @@
       <c r="A40" s="20" t="n">
         <v>17</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="32" t="n">
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="31" t="n">
         <v>70</v>
       </c>
       <c r="G40" s="23" t="s">
@@ -2675,16 +2322,16 @@
       <c r="K40" s="26"/>
       <c r="L40" s="26"/>
       <c r="M40" s="26"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
-      <c r="P40" s="32" t="n">
+      <c r="N40" s="31"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="31" t="n">
         <v>45</v>
       </c>
-      <c r="Q40" s="32" t="n">
+      <c r="Q40" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="R40" s="32"/>
-      <c r="S40" s="30"/>
+      <c r="R40" s="31"/>
+      <c r="S40" s="25"/>
       <c r="T40" s="26"/>
       <c r="U40" s="21" t="n">
         <f aca="false">SUM(H40:S40)</f>
@@ -2695,13 +2342,13 @@
       <c r="A41" s="20" t="n">
         <v>18</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="32" t="n">
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="31" t="n">
         <v>40</v>
       </c>
       <c r="G41" s="23" t="s">
@@ -2713,16 +2360,16 @@
       <c r="K41" s="26"/>
       <c r="L41" s="26"/>
       <c r="M41" s="26"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="32"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="32" t="n">
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31" t="n">
         <v>25</v>
       </c>
-      <c r="R41" s="32" t="n">
+      <c r="R41" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="S41" s="30"/>
+      <c r="S41" s="25"/>
       <c r="T41" s="26"/>
       <c r="U41" s="21" t="n">
         <f aca="false">SUM(H41:S41)</f>
@@ -2758,13 +2405,13 @@
       <c r="A43" s="20" t="n">
         <v>19</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="32" t="n">
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="31" t="n">
         <v>40</v>
       </c>
       <c r="G43" s="23" t="s">
@@ -2776,14 +2423,14 @@
       <c r="K43" s="26"/>
       <c r="L43" s="26"/>
       <c r="M43" s="26"/>
-      <c r="N43" s="32" t="n">
+      <c r="N43" s="31" t="n">
         <v>40</v>
       </c>
-      <c r="O43" s="32"/>
-      <c r="P43" s="32"/>
-      <c r="Q43" s="32"/>
-      <c r="R43" s="32"/>
-      <c r="S43" s="30"/>
+      <c r="O43" s="31"/>
+      <c r="P43" s="31"/>
+      <c r="Q43" s="31"/>
+      <c r="R43" s="31"/>
+      <c r="S43" s="25"/>
       <c r="T43" s="26"/>
       <c r="U43" s="21" t="n">
         <f aca="false">SUM(H43:S43)</f>
@@ -2819,13 +2466,13 @@
       <c r="A45" s="20" t="n">
         <v>20</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="32" t="n">
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="31" t="n">
         <v>40</v>
       </c>
       <c r="G45" s="23" t="s">
@@ -2837,16 +2484,16 @@
       <c r="K45" s="26"/>
       <c r="L45" s="26"/>
       <c r="M45" s="26"/>
-      <c r="N45" s="32" t="n">
+      <c r="N45" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="O45" s="32" t="n">
+      <c r="O45" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="P45" s="32"/>
-      <c r="Q45" s="32"/>
-      <c r="R45" s="32"/>
-      <c r="S45" s="30"/>
+      <c r="P45" s="31"/>
+      <c r="Q45" s="31"/>
+      <c r="R45" s="31"/>
+      <c r="S45" s="25"/>
       <c r="T45" s="26"/>
       <c r="U45" s="21" t="n">
         <f aca="false">SUM(H45:S45)</f>
@@ -2857,13 +2504,13 @@
       <c r="A46" s="20" t="n">
         <v>21</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="32" t="n">
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="31" t="n">
         <v>20</v>
       </c>
       <c r="G46" s="23" t="s">
@@ -2875,16 +2522,16 @@
       <c r="K46" s="26"/>
       <c r="L46" s="26"/>
       <c r="M46" s="26"/>
-      <c r="N46" s="32"/>
-      <c r="O46" s="32" t="n">
+      <c r="N46" s="31"/>
+      <c r="O46" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="P46" s="32" t="n">
+      <c r="P46" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="Q46" s="32"/>
-      <c r="R46" s="32"/>
-      <c r="S46" s="30"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="31"/>
+      <c r="S46" s="25"/>
       <c r="T46" s="26"/>
       <c r="U46" s="21" t="n">
         <f aca="false">SUM(H46:S46)</f>
@@ -2920,13 +2567,13 @@
       <c r="A48" s="20" t="n">
         <v>22</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="32" t="n">
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="31" t="n">
         <v>15</v>
       </c>
       <c r="G48" s="23" t="s">
@@ -2938,14 +2585,14 @@
       <c r="K48" s="26"/>
       <c r="L48" s="26"/>
       <c r="M48" s="26"/>
-      <c r="N48" s="32"/>
-      <c r="O48" s="32"/>
-      <c r="P48" s="32"/>
-      <c r="Q48" s="32" t="n">
+      <c r="N48" s="31"/>
+      <c r="O48" s="31"/>
+      <c r="P48" s="31"/>
+      <c r="Q48" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="R48" s="32"/>
-      <c r="S48" s="30"/>
+      <c r="R48" s="31"/>
+      <c r="S48" s="25"/>
       <c r="T48" s="26"/>
       <c r="U48" s="21" t="n">
         <f aca="false">SUM(H48:S48)</f>
@@ -2956,13 +2603,13 @@
       <c r="A49" s="20" t="n">
         <v>23</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="32" t="n">
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="31" t="n">
         <v>30</v>
       </c>
       <c r="G49" s="23" t="s">
@@ -2974,16 +2621,16 @@
       <c r="K49" s="26"/>
       <c r="L49" s="26"/>
       <c r="M49" s="26"/>
-      <c r="N49" s="32"/>
-      <c r="O49" s="32"/>
-      <c r="P49" s="32" t="n">
+      <c r="N49" s="31"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="Q49" s="32" t="n">
+      <c r="Q49" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="R49" s="32"/>
-      <c r="S49" s="30"/>
+      <c r="R49" s="31"/>
+      <c r="S49" s="25"/>
       <c r="T49" s="26"/>
       <c r="U49" s="21" t="n">
         <f aca="false">SUM(H49:S49)</f>
@@ -2994,13 +2641,13 @@
       <c r="A50" s="20" t="n">
         <v>24</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="32" t="n">
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="31" t="n">
         <v>30</v>
       </c>
       <c r="G50" s="23" t="s">
@@ -3012,16 +2659,16 @@
       <c r="K50" s="26"/>
       <c r="L50" s="26"/>
       <c r="M50" s="26"/>
-      <c r="N50" s="32"/>
-      <c r="O50" s="32"/>
-      <c r="P50" s="32" t="n">
+      <c r="N50" s="31"/>
+      <c r="O50" s="31"/>
+      <c r="P50" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="Q50" s="32" t="n">
+      <c r="Q50" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="R50" s="32"/>
-      <c r="S50" s="30"/>
+      <c r="R50" s="31"/>
+      <c r="S50" s="25"/>
       <c r="T50" s="26"/>
       <c r="U50" s="21" t="n">
         <f aca="false">SUM(H50:S50)</f>
@@ -3057,13 +2704,13 @@
       <c r="A52" s="20" t="n">
         <v>25</v>
       </c>
-      <c r="B52" s="31" t="s">
+      <c r="B52" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="32" t="n">
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="31" t="n">
         <v>20</v>
       </c>
       <c r="G52" s="23" t="s">
@@ -3075,14 +2722,14 @@
       <c r="K52" s="26"/>
       <c r="L52" s="26"/>
       <c r="M52" s="26"/>
-      <c r="N52" s="32"/>
-      <c r="O52" s="32" t="n">
+      <c r="N52" s="31"/>
+      <c r="O52" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="P52" s="32"/>
-      <c r="Q52" s="32"/>
-      <c r="R52" s="32"/>
-      <c r="S52" s="30"/>
+      <c r="P52" s="31"/>
+      <c r="Q52" s="31"/>
+      <c r="R52" s="31"/>
+      <c r="S52" s="25"/>
       <c r="T52" s="26"/>
       <c r="U52" s="21" t="n">
         <f aca="false">SUM(H52:S52)</f>
@@ -3118,13 +2765,13 @@
       <c r="A54" s="20" t="n">
         <v>26</v>
       </c>
-      <c r="B54" s="31" t="s">
+      <c r="B54" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="32" t="n">
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="31" t="n">
         <v>10</v>
       </c>
       <c r="G54" s="22" t="s">
@@ -3136,14 +2783,14 @@
       <c r="K54" s="26"/>
       <c r="L54" s="26"/>
       <c r="M54" s="26"/>
-      <c r="N54" s="32"/>
-      <c r="O54" s="32"/>
-      <c r="P54" s="32" t="n">
+      <c r="N54" s="31"/>
+      <c r="O54" s="31"/>
+      <c r="P54" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="Q54" s="32"/>
-      <c r="R54" s="32"/>
-      <c r="S54" s="30"/>
+      <c r="Q54" s="31"/>
+      <c r="R54" s="31"/>
+      <c r="S54" s="25"/>
       <c r="T54" s="26"/>
       <c r="U54" s="21" t="n">
         <f aca="false">SUM(H54:S54)</f>
@@ -3154,13 +2801,13 @@
       <c r="A55" s="20" t="n">
         <v>27</v>
       </c>
-      <c r="B55" s="31" t="s">
+      <c r="B55" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="32" t="n">
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="31" t="n">
         <v>30</v>
       </c>
       <c r="G55" s="22" t="s">
@@ -3172,14 +2819,14 @@
       <c r="K55" s="26"/>
       <c r="L55" s="26"/>
       <c r="M55" s="26"/>
-      <c r="N55" s="32"/>
-      <c r="O55" s="32"/>
-      <c r="P55" s="32"/>
-      <c r="Q55" s="32"/>
-      <c r="R55" s="32" t="n">
+      <c r="N55" s="31"/>
+      <c r="O55" s="31"/>
+      <c r="P55" s="31"/>
+      <c r="Q55" s="31"/>
+      <c r="R55" s="31" t="n">
         <v>30</v>
       </c>
-      <c r="S55" s="30"/>
+      <c r="S55" s="25"/>
       <c r="T55" s="26"/>
       <c r="U55" s="21" t="n">
         <f aca="false">SUM(H55:S55)</f>
@@ -3215,13 +2862,13 @@
       <c r="A57" s="20" t="n">
         <v>28</v>
       </c>
-      <c r="B57" s="31" t="s">
+      <c r="B57" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="32" t="n">
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="30"/>
+      <c r="F57" s="31" t="n">
         <v>70</v>
       </c>
       <c r="G57" s="22" t="s">
@@ -3233,14 +2880,14 @@
       <c r="K57" s="26"/>
       <c r="L57" s="26"/>
       <c r="M57" s="26"/>
-      <c r="N57" s="32"/>
-      <c r="O57" s="32"/>
-      <c r="P57" s="32"/>
-      <c r="Q57" s="32"/>
-      <c r="R57" s="32" t="n">
+      <c r="N57" s="31"/>
+      <c r="O57" s="31"/>
+      <c r="P57" s="31"/>
+      <c r="Q57" s="31"/>
+      <c r="R57" s="31" t="n">
         <v>70</v>
       </c>
-      <c r="S57" s="30"/>
+      <c r="S57" s="25"/>
       <c r="T57" s="26"/>
       <c r="U57" s="21" t="n">
         <f aca="false">SUM(H57:S57)</f>
@@ -3251,13 +2898,13 @@
       <c r="A58" s="20" t="n">
         <v>29</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="31"/>
-      <c r="F58" s="32" t="n">
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="31" t="n">
         <v>20</v>
       </c>
       <c r="G58" s="22" t="s">
@@ -3269,12 +2916,12 @@
       <c r="K58" s="26"/>
       <c r="L58" s="26"/>
       <c r="M58" s="26"/>
-      <c r="N58" s="32"/>
-      <c r="O58" s="32"/>
-      <c r="P58" s="32"/>
-      <c r="Q58" s="32"/>
-      <c r="R58" s="32"/>
-      <c r="S58" s="30" t="n">
+      <c r="N58" s="31"/>
+      <c r="O58" s="31"/>
+      <c r="P58" s="31"/>
+      <c r="Q58" s="31"/>
+      <c r="R58" s="31"/>
+      <c r="S58" s="25" t="n">
         <v>20</v>
       </c>
       <c r="T58" s="26"/>
@@ -3287,13 +2934,13 @@
       <c r="A59" s="20" t="n">
         <v>30</v>
       </c>
-      <c r="B59" s="31" t="s">
+      <c r="B59" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="32" t="n">
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="31" t="n">
         <v>20</v>
       </c>
       <c r="G59" s="22" t="s">
@@ -3305,16 +2952,16 @@
       <c r="K59" s="26"/>
       <c r="L59" s="26"/>
       <c r="M59" s="26"/>
-      <c r="N59" s="32"/>
-      <c r="O59" s="32"/>
-      <c r="P59" s="32"/>
-      <c r="Q59" s="32" t="n">
+      <c r="N59" s="31"/>
+      <c r="O59" s="31"/>
+      <c r="P59" s="31"/>
+      <c r="Q59" s="31" t="n">
         <v>5</v>
       </c>
-      <c r="R59" s="32" t="n">
+      <c r="R59" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="S59" s="30"/>
+      <c r="S59" s="25"/>
       <c r="T59" s="26"/>
       <c r="U59" s="21" t="n">
         <f aca="false">SUM(H59:S59)</f>
@@ -3325,16 +2972,16 @@
       <c r="A60" s="20" t="n">
         <v>33</v>
       </c>
-      <c r="B60" s="31" t="s">
+      <c r="B60" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="32" t="n">
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="31" t="n">
         <v>20</v>
       </c>
-      <c r="G60" s="32" t="s">
+      <c r="G60" s="31" t="s">
         <v>19</v>
       </c>
       <c r="H60" s="26"/>
@@ -3343,22 +2990,22 @@
       <c r="K60" s="26"/>
       <c r="L60" s="26"/>
       <c r="M60" s="26"/>
-      <c r="N60" s="32" t="n">
+      <c r="N60" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="O60" s="32" t="n">
+      <c r="O60" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="P60" s="32" t="n">
+      <c r="P60" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="Q60" s="32" t="n">
+      <c r="Q60" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="R60" s="32" t="n">
+      <c r="R60" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="S60" s="30"/>
+      <c r="S60" s="25"/>
       <c r="T60" s="26"/>
       <c r="U60" s="21" t="n">
         <f aca="false">SUM(H60:S60)</f>
@@ -3394,16 +3041,16 @@
       <c r="A62" s="20" t="n">
         <v>32</v>
       </c>
-      <c r="B62" s="31" t="s">
+      <c r="B62" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C62" s="31"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="32" t="n">
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="31" t="n">
         <v>35</v>
       </c>
-      <c r="G62" s="32" t="s">
+      <c r="G62" s="31" t="s">
         <v>19</v>
       </c>
       <c r="H62" s="26"/>
@@ -3412,22 +3059,22 @@
       <c r="K62" s="26"/>
       <c r="L62" s="26"/>
       <c r="M62" s="26"/>
-      <c r="N62" s="32" t="n">
+      <c r="N62" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="O62" s="32" t="n">
+      <c r="O62" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="P62" s="32" t="n">
+      <c r="P62" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="Q62" s="32" t="n">
+      <c r="Q62" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="R62" s="32" t="n">
+      <c r="R62" s="31" t="n">
         <v>7</v>
       </c>
-      <c r="S62" s="30"/>
+      <c r="S62" s="25"/>
       <c r="T62" s="26"/>
       <c r="U62" s="21" t="n">
         <f aca="false">SUM(H62:S62)</f>
@@ -3436,44 +3083,44 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="20"/>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="32" t="n">
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="31" t="n">
         <f aca="false">(900-SUM(F28:F62))</f>
         <v>95</v>
       </c>
-      <c r="G63" s="32"/>
+      <c r="G63" s="31"/>
       <c r="H63" s="26"/>
       <c r="I63" s="26"/>
       <c r="J63" s="26"/>
       <c r="K63" s="26"/>
       <c r="L63" s="26"/>
       <c r="M63" s="26"/>
-      <c r="N63" s="32" t="n">
+      <c r="N63" s="31" t="n">
         <f aca="false">(180-SUM(N28:N62))</f>
         <v>19</v>
       </c>
-      <c r="O63" s="32" t="n">
+      <c r="O63" s="31" t="n">
         <f aca="false">(180-SUM(O28:O62))</f>
         <v>24</v>
       </c>
-      <c r="P63" s="32" t="n">
+      <c r="P63" s="31" t="n">
         <f aca="false">(180-SUM(P28:P62))</f>
         <v>19</v>
       </c>
-      <c r="Q63" s="32" t="n">
+      <c r="Q63" s="31" t="n">
         <f aca="false">(180-SUM(Q28:Q62))</f>
         <v>14</v>
       </c>
-      <c r="R63" s="32" t="n">
+      <c r="R63" s="31" t="n">
         <f aca="false">(158-SUM(R28:R62))</f>
         <v>17</v>
       </c>
-      <c r="S63" s="32" t="n">
+      <c r="S63" s="31" t="n">
         <f aca="false">(22-SUM(S28:S62))</f>
         <v>2</v>
       </c>
@@ -3485,44 +3132,44 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="20"/>
-      <c r="B64" s="31" t="s">
+      <c r="B64" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="31"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="31"/>
-      <c r="F64" s="32" t="n">
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="31" t="n">
         <f aca="false">SUM(F28:F63)</f>
         <v>900</v>
       </c>
-      <c r="G64" s="32"/>
+      <c r="G64" s="31"/>
       <c r="H64" s="26"/>
       <c r="I64" s="26"/>
       <c r="J64" s="26"/>
       <c r="K64" s="26"/>
       <c r="L64" s="26"/>
       <c r="M64" s="26"/>
-      <c r="N64" s="32" t="n">
+      <c r="N64" s="31" t="n">
         <f aca="false">SUM(N28:N63)</f>
         <v>180</v>
       </c>
-      <c r="O64" s="32" t="n">
+      <c r="O64" s="31" t="n">
         <f aca="false">SUM(O28:O63)</f>
         <v>180</v>
       </c>
-      <c r="P64" s="32" t="n">
+      <c r="P64" s="31" t="n">
         <f aca="false">SUM(P28:P63)</f>
         <v>180</v>
       </c>
-      <c r="Q64" s="32" t="n">
+      <c r="Q64" s="31" t="n">
         <f aca="false">SUM(Q28:Q63)</f>
         <v>180</v>
       </c>
-      <c r="R64" s="32" t="n">
+      <c r="R64" s="31" t="n">
         <f aca="false">SUM(R28:R63)</f>
         <v>158</v>
       </c>
-      <c r="S64" s="32" t="n">
+      <c r="S64" s="31" t="n">
         <f aca="false">SUM(S28:S63)</f>
         <v>22</v>
       </c>
@@ -3534,44 +3181,44 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="20"/>
-      <c r="B65" s="34" t="s">
+      <c r="B65" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="35" t="n">
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="34" t="n">
         <f aca="false">SUM(F24,F64)</f>
         <v>1120</v>
       </c>
-      <c r="G65" s="35"/>
+      <c r="G65" s="34"/>
       <c r="H65" s="26"/>
       <c r="I65" s="26"/>
       <c r="J65" s="26"/>
       <c r="K65" s="26"/>
       <c r="L65" s="26"/>
       <c r="M65" s="26"/>
-      <c r="N65" s="35" t="n">
+      <c r="N65" s="34" t="n">
         <f aca="false">SUM(N18:N23,N28:N63)</f>
         <v>180</v>
       </c>
-      <c r="O65" s="35" t="n">
+      <c r="O65" s="34" t="n">
         <f aca="false">SUM(O18:O23,O28:O63)</f>
         <v>180</v>
       </c>
-      <c r="P65" s="35" t="n">
+      <c r="P65" s="34" t="n">
         <f aca="false">SUM(P18:P23,P28:P63)</f>
         <v>180</v>
       </c>
-      <c r="Q65" s="35" t="n">
+      <c r="Q65" s="34" t="n">
         <f aca="false">SUM(Q18:Q23,Q28:Q63)</f>
         <v>180</v>
       </c>
-      <c r="R65" s="35" t="n">
+      <c r="R65" s="34" t="n">
         <f aca="false">SUM(R18:R23,R28:R63)</f>
         <v>158</v>
       </c>
-      <c r="S65" s="35" t="n">
+      <c r="S65" s="34" t="n">
         <f aca="false">SUM(S18:S23,S28:S63)</f>
         <v>22</v>
       </c>
@@ -3612,14 +3259,14 @@
       <c r="A67" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="36" t="s">
+      <c r="B67" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="36"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="35"/>
+      <c r="F67" s="35"/>
+      <c r="G67" s="35"/>
       <c r="H67" s="20" t="n">
         <v>40</v>
       </c>
@@ -3665,348 +3312,348 @@
       <c r="A68" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="B68" s="37" t="s">
+      <c r="B68" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="C68" s="37"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="37"/>
-      <c r="G68" s="37"/>
-      <c r="H68" s="38"/>
-      <c r="I68" s="38"/>
-      <c r="J68" s="38"/>
-      <c r="K68" s="38"/>
-      <c r="L68" s="38" t="s">
+      <c r="C68" s="36"/>
+      <c r="D68" s="36"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="36"/>
+      <c r="G68" s="36"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="M68" s="38"/>
-      <c r="N68" s="39"/>
-      <c r="O68" s="39"/>
-      <c r="P68" s="39"/>
-      <c r="Q68" s="39"/>
-      <c r="R68" s="39"/>
-      <c r="S68" s="38"/>
-      <c r="T68" s="38"/>
+      <c r="M68" s="37"/>
+      <c r="N68" s="38"/>
+      <c r="O68" s="38"/>
+      <c r="P68" s="38"/>
+      <c r="Q68" s="38"/>
+      <c r="R68" s="38"/>
+      <c r="S68" s="37"/>
+      <c r="T68" s="37"/>
       <c r="U68" s="29"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="B69" s="37" t="s">
+      <c r="B69" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="C69" s="37"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="37"/>
-      <c r="F69" s="37"/>
-      <c r="G69" s="37"/>
-      <c r="H69" s="38"/>
-      <c r="I69" s="38"/>
-      <c r="J69" s="38"/>
-      <c r="K69" s="38"/>
-      <c r="L69" s="38"/>
-      <c r="M69" s="38" t="s">
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37"/>
+      <c r="K69" s="37"/>
+      <c r="L69" s="37"/>
+      <c r="M69" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="N69" s="39"/>
-      <c r="O69" s="39"/>
-      <c r="P69" s="39"/>
-      <c r="Q69" s="39"/>
-      <c r="R69" s="39"/>
-      <c r="S69" s="38"/>
-      <c r="T69" s="38"/>
+      <c r="N69" s="38"/>
+      <c r="O69" s="38"/>
+      <c r="P69" s="38"/>
+      <c r="Q69" s="38"/>
+      <c r="R69" s="38"/>
+      <c r="S69" s="37"/>
+      <c r="T69" s="37"/>
       <c r="U69" s="21"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="B70" s="37" t="s">
+      <c r="B70" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="C70" s="37"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="37"/>
-      <c r="G70" s="37"/>
-      <c r="H70" s="38"/>
-      <c r="I70" s="38"/>
-      <c r="J70" s="38"/>
-      <c r="K70" s="38"/>
-      <c r="L70" s="38"/>
-      <c r="M70" s="38"/>
-      <c r="N70" s="39"/>
-      <c r="O70" s="39" t="s">
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36"/>
+      <c r="F70" s="36"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="37"/>
+      <c r="K70" s="37"/>
+      <c r="L70" s="37"/>
+      <c r="M70" s="37"/>
+      <c r="N70" s="38"/>
+      <c r="O70" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="P70" s="39"/>
-      <c r="Q70" s="39"/>
-      <c r="R70" s="39"/>
-      <c r="S70" s="38"/>
-      <c r="T70" s="38"/>
+      <c r="P70" s="38"/>
+      <c r="Q70" s="38"/>
+      <c r="R70" s="38"/>
+      <c r="S70" s="37"/>
+      <c r="T70" s="37"/>
       <c r="U70" s="21"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="B71" s="37" t="s">
+      <c r="B71" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="C71" s="37"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="37"/>
-      <c r="H71" s="38"/>
-      <c r="I71" s="38"/>
-      <c r="J71" s="38"/>
-      <c r="K71" s="38"/>
-      <c r="L71" s="38"/>
-      <c r="M71" s="38"/>
-      <c r="N71" s="39"/>
-      <c r="O71" s="39"/>
-      <c r="P71" s="39" t="s">
+      <c r="C71" s="36"/>
+      <c r="D71" s="36"/>
+      <c r="E71" s="36"/>
+      <c r="F71" s="36"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
+      <c r="J71" s="37"/>
+      <c r="K71" s="37"/>
+      <c r="L71" s="37"/>
+      <c r="M71" s="37"/>
+      <c r="N71" s="38"/>
+      <c r="O71" s="38"/>
+      <c r="P71" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="Q71" s="39"/>
-      <c r="R71" s="39"/>
-      <c r="S71" s="38"/>
-      <c r="T71" s="38"/>
+      <c r="Q71" s="38"/>
+      <c r="R71" s="38"/>
+      <c r="S71" s="37"/>
+      <c r="T71" s="37"/>
       <c r="U71" s="29"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="B72" s="37" t="s">
+      <c r="B72" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="C72" s="37"/>
-      <c r="D72" s="37"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="37"/>
-      <c r="H72" s="38"/>
-      <c r="I72" s="38"/>
-      <c r="J72" s="38"/>
-      <c r="K72" s="38"/>
-      <c r="L72" s="38"/>
-      <c r="M72" s="38"/>
-      <c r="N72" s="40"/>
-      <c r="O72" s="40"/>
-      <c r="P72" s="40" t="s">
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="37"/>
+      <c r="I72" s="37"/>
+      <c r="J72" s="37"/>
+      <c r="K72" s="37"/>
+      <c r="L72" s="37"/>
+      <c r="M72" s="37"/>
+      <c r="N72" s="39"/>
+      <c r="O72" s="39"/>
+      <c r="P72" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="Q72" s="40"/>
-      <c r="R72" s="40"/>
-      <c r="S72" s="38"/>
-      <c r="T72" s="38"/>
+      <c r="Q72" s="39"/>
+      <c r="R72" s="39"/>
+      <c r="S72" s="37"/>
+      <c r="T72" s="37"/>
       <c r="U72" s="21"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="B73" s="37" t="s">
+      <c r="B73" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C73" s="37"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="37"/>
-      <c r="G73" s="37"/>
-      <c r="H73" s="38"/>
-      <c r="I73" s="38"/>
-      <c r="J73" s="38"/>
-      <c r="K73" s="38"/>
-      <c r="L73" s="38"/>
-      <c r="M73" s="38"/>
-      <c r="N73" s="39"/>
-      <c r="O73" s="39"/>
-      <c r="P73" s="39" t="s">
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="36"/>
+      <c r="G73" s="36"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="37"/>
+      <c r="K73" s="37"/>
+      <c r="L73" s="37"/>
+      <c r="M73" s="37"/>
+      <c r="N73" s="38"/>
+      <c r="O73" s="38"/>
+      <c r="P73" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="Q73" s="39"/>
-      <c r="R73" s="39"/>
-      <c r="S73" s="38"/>
-      <c r="T73" s="38"/>
+      <c r="Q73" s="38"/>
+      <c r="R73" s="38"/>
+      <c r="S73" s="37"/>
+      <c r="T73" s="37"/>
       <c r="U73" s="29"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="20" t="n">
         <v>7</v>
       </c>
-      <c r="B74" s="37" t="s">
+      <c r="B74" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="C74" s="37"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="37"/>
-      <c r="H74" s="38"/>
-      <c r="I74" s="38"/>
-      <c r="J74" s="38"/>
-      <c r="K74" s="38"/>
-      <c r="L74" s="38"/>
-      <c r="M74" s="38"/>
-      <c r="N74" s="40"/>
-      <c r="O74" s="40"/>
-      <c r="P74" s="40" t="s">
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
+      <c r="J74" s="37"/>
+      <c r="K74" s="37"/>
+      <c r="L74" s="37"/>
+      <c r="M74" s="37"/>
+      <c r="N74" s="39"/>
+      <c r="O74" s="39"/>
+      <c r="P74" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="Q74" s="40"/>
-      <c r="R74" s="40"/>
-      <c r="S74" s="38"/>
-      <c r="T74" s="38"/>
+      <c r="Q74" s="39"/>
+      <c r="R74" s="39"/>
+      <c r="S74" s="37"/>
+      <c r="T74" s="37"/>
       <c r="U74" s="21"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="B75" s="37" t="s">
+      <c r="B75" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="C75" s="37"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="37"/>
-      <c r="F75" s="37"/>
-      <c r="G75" s="37"/>
-      <c r="H75" s="38"/>
-      <c r="I75" s="38"/>
-      <c r="J75" s="38"/>
-      <c r="K75" s="38"/>
-      <c r="L75" s="38"/>
-      <c r="M75" s="38"/>
-      <c r="N75" s="40"/>
-      <c r="O75" s="40"/>
-      <c r="P75" s="40"/>
-      <c r="Q75" s="40" t="s">
+      <c r="C75" s="36"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="37"/>
+      <c r="J75" s="37"/>
+      <c r="K75" s="37"/>
+      <c r="L75" s="37"/>
+      <c r="M75" s="37"/>
+      <c r="N75" s="39"/>
+      <c r="O75" s="39"/>
+      <c r="P75" s="39"/>
+      <c r="Q75" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="R75" s="40"/>
-      <c r="S75" s="38"/>
-      <c r="T75" s="38"/>
+      <c r="R75" s="39"/>
+      <c r="S75" s="37"/>
+      <c r="T75" s="37"/>
       <c r="U75" s="21"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="20" t="n">
         <v>9</v>
       </c>
-      <c r="B76" s="37" t="s">
+      <c r="B76" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="C76" s="37"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="37"/>
-      <c r="H76" s="38"/>
-      <c r="I76" s="38"/>
-      <c r="J76" s="38"/>
-      <c r="K76" s="38"/>
-      <c r="L76" s="38"/>
-      <c r="M76" s="38"/>
-      <c r="N76" s="40"/>
-      <c r="O76" s="40"/>
-      <c r="P76" s="40"/>
-      <c r="Q76" s="40" t="s">
+      <c r="C76" s="36"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="36"/>
+      <c r="F76" s="36"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="37"/>
+      <c r="I76" s="37"/>
+      <c r="J76" s="37"/>
+      <c r="K76" s="37"/>
+      <c r="L76" s="37"/>
+      <c r="M76" s="37"/>
+      <c r="N76" s="39"/>
+      <c r="O76" s="39"/>
+      <c r="P76" s="39"/>
+      <c r="Q76" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="R76" s="40"/>
-      <c r="S76" s="38"/>
-      <c r="T76" s="38"/>
+      <c r="R76" s="39"/>
+      <c r="S76" s="37"/>
+      <c r="T76" s="37"/>
       <c r="U76" s="21"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="B77" s="37" t="s">
+      <c r="B77" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="C77" s="37"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="37"/>
-      <c r="G77" s="37"/>
-      <c r="H77" s="38"/>
-      <c r="I77" s="38"/>
-      <c r="J77" s="38"/>
-      <c r="K77" s="38"/>
-      <c r="L77" s="38"/>
-      <c r="M77" s="38"/>
-      <c r="N77" s="40"/>
-      <c r="O77" s="40"/>
-      <c r="P77" s="40"/>
-      <c r="Q77" s="40" t="s">
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="36"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="37"/>
+      <c r="I77" s="37"/>
+      <c r="J77" s="37"/>
+      <c r="K77" s="37"/>
+      <c r="L77" s="37"/>
+      <c r="M77" s="37"/>
+      <c r="N77" s="39"/>
+      <c r="O77" s="39"/>
+      <c r="P77" s="39"/>
+      <c r="Q77" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="R77" s="40"/>
-      <c r="S77" s="38"/>
-      <c r="T77" s="38"/>
+      <c r="R77" s="39"/>
+      <c r="S77" s="37"/>
+      <c r="T77" s="37"/>
       <c r="U77" s="21"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="20" t="n">
         <v>11</v>
       </c>
-      <c r="B78" s="37" t="s">
+      <c r="B78" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C78" s="37"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="37"/>
-      <c r="G78" s="37"/>
-      <c r="H78" s="38"/>
-      <c r="I78" s="38"/>
-      <c r="J78" s="38"/>
-      <c r="K78" s="38"/>
-      <c r="L78" s="38"/>
-      <c r="M78" s="38"/>
-      <c r="N78" s="39"/>
-      <c r="O78" s="39"/>
-      <c r="P78" s="39"/>
-      <c r="Q78" s="39"/>
-      <c r="R78" s="39" t="s">
+      <c r="C78" s="36"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="36"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37"/>
+      <c r="J78" s="37"/>
+      <c r="K78" s="37"/>
+      <c r="L78" s="37"/>
+      <c r="M78" s="37"/>
+      <c r="N78" s="38"/>
+      <c r="O78" s="38"/>
+      <c r="P78" s="38"/>
+      <c r="Q78" s="38"/>
+      <c r="R78" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="S78" s="38"/>
-      <c r="T78" s="38"/>
+      <c r="S78" s="37"/>
+      <c r="T78" s="37"/>
       <c r="U78" s="29"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="20" t="n">
         <v>12</v>
       </c>
-      <c r="B79" s="37" t="s">
+      <c r="B79" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="C79" s="37"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="37"/>
-      <c r="F79" s="37"/>
-      <c r="G79" s="37"/>
-      <c r="H79" s="38"/>
-      <c r="I79" s="38"/>
-      <c r="J79" s="38"/>
-      <c r="K79" s="38"/>
-      <c r="L79" s="38"/>
-      <c r="M79" s="38"/>
-      <c r="N79" s="39"/>
-      <c r="O79" s="39"/>
-      <c r="P79" s="39"/>
-      <c r="Q79" s="39"/>
-      <c r="R79" s="39" t="s">
+      <c r="C79" s="36"/>
+      <c r="D79" s="36"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="36"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="37"/>
+      <c r="I79" s="37"/>
+      <c r="J79" s="37"/>
+      <c r="K79" s="37"/>
+      <c r="L79" s="37"/>
+      <c r="M79" s="37"/>
+      <c r="N79" s="38"/>
+      <c r="O79" s="38"/>
+      <c r="P79" s="38"/>
+      <c r="Q79" s="38"/>
+      <c r="R79" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="S79" s="38"/>
-      <c r="T79" s="38"/>
+      <c r="S79" s="37"/>
+      <c r="T79" s="37"/>
       <c r="U79" s="21"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4044,251 +3691,251 @@
       <c r="A81" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B81" s="36" t="s">
+      <c r="B81" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C81" s="36"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-      <c r="F81" s="36"/>
-      <c r="G81" s="36"/>
-      <c r="H81" s="41" t="n">
+      <c r="C81" s="35"/>
+      <c r="D81" s="35"/>
+      <c r="E81" s="35"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="35"/>
+      <c r="H81" s="40" t="n">
         <v>40</v>
       </c>
-      <c r="I81" s="41" t="n">
+      <c r="I81" s="40" t="n">
         <v>41</v>
       </c>
-      <c r="J81" s="41" t="n">
+      <c r="J81" s="40" t="n">
         <v>42</v>
       </c>
-      <c r="K81" s="41" t="n">
+      <c r="K81" s="40" t="n">
         <v>43</v>
       </c>
-      <c r="L81" s="41" t="n">
+      <c r="L81" s="40" t="n">
         <v>44</v>
       </c>
-      <c r="M81" s="41" t="n">
+      <c r="M81" s="40" t="n">
         <v>45</v>
       </c>
-      <c r="N81" s="41" t="n">
+      <c r="N81" s="40" t="n">
         <v>46</v>
       </c>
-      <c r="O81" s="41" t="n">
+      <c r="O81" s="40" t="n">
         <v>47</v>
       </c>
-      <c r="P81" s="41" t="n">
+      <c r="P81" s="40" t="n">
         <v>48</v>
       </c>
-      <c r="Q81" s="41" t="n">
+      <c r="Q81" s="40" t="n">
         <v>49</v>
       </c>
-      <c r="R81" s="41" t="n">
+      <c r="R81" s="40" t="n">
         <v>50</v>
       </c>
-      <c r="S81" s="41" t="n">
+      <c r="S81" s="40" t="n">
         <v>51</v>
       </c>
-      <c r="T81" s="41" t="n">
+      <c r="T81" s="40" t="n">
         <v>52</v>
       </c>
-      <c r="U81" s="42"/>
+      <c r="U81" s="41"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="B82" s="37" t="s">
+      <c r="B82" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="37"/>
-      <c r="G82" s="37"/>
-      <c r="H82" s="38"/>
-      <c r="I82" s="38"/>
-      <c r="J82" s="38"/>
-      <c r="K82" s="38"/>
-      <c r="L82" s="38"/>
-      <c r="M82" s="38"/>
-      <c r="N82" s="39"/>
-      <c r="O82" s="39"/>
-      <c r="P82" s="39"/>
-      <c r="Q82" s="39"/>
-      <c r="R82" s="39"/>
-      <c r="S82" s="38"/>
-      <c r="T82" s="38"/>
-      <c r="U82" s="43"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="36"/>
+      <c r="E82" s="36"/>
+      <c r="F82" s="36"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="37"/>
+      <c r="I82" s="37"/>
+      <c r="J82" s="37"/>
+      <c r="K82" s="37"/>
+      <c r="L82" s="37"/>
+      <c r="M82" s="37"/>
+      <c r="N82" s="38"/>
+      <c r="O82" s="38"/>
+      <c r="P82" s="38"/>
+      <c r="Q82" s="38"/>
+      <c r="R82" s="38"/>
+      <c r="S82" s="37"/>
+      <c r="T82" s="37"/>
+      <c r="U82" s="42"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="B83" s="37" t="s">
+      <c r="B83" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="C83" s="37"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="37"/>
-      <c r="G83" s="37"/>
-      <c r="H83" s="38"/>
-      <c r="I83" s="38"/>
-      <c r="J83" s="38"/>
-      <c r="K83" s="38"/>
-      <c r="L83" s="38"/>
-      <c r="M83" s="38"/>
-      <c r="N83" s="39"/>
-      <c r="O83" s="39"/>
-      <c r="P83" s="39"/>
-      <c r="Q83" s="39"/>
-      <c r="R83" s="39"/>
-      <c r="S83" s="38"/>
-      <c r="T83" s="38"/>
-      <c r="U83" s="42"/>
+      <c r="C83" s="36"/>
+      <c r="D83" s="36"/>
+      <c r="E83" s="36"/>
+      <c r="F83" s="36"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="37"/>
+      <c r="J83" s="37"/>
+      <c r="K83" s="37"/>
+      <c r="L83" s="37"/>
+      <c r="M83" s="37"/>
+      <c r="N83" s="38"/>
+      <c r="O83" s="38"/>
+      <c r="P83" s="38"/>
+      <c r="Q83" s="38"/>
+      <c r="R83" s="38"/>
+      <c r="S83" s="37"/>
+      <c r="T83" s="37"/>
+      <c r="U83" s="41"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="B84" s="37" t="s">
+      <c r="B84" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="C84" s="37"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="37"/>
-      <c r="G84" s="37"/>
-      <c r="H84" s="38"/>
-      <c r="I84" s="38" t="s">
+      <c r="C84" s="36"/>
+      <c r="D84" s="36"/>
+      <c r="E84" s="36"/>
+      <c r="F84" s="36"/>
+      <c r="G84" s="36"/>
+      <c r="H84" s="37"/>
+      <c r="I84" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="J84" s="38"/>
-      <c r="K84" s="38"/>
-      <c r="L84" s="38"/>
-      <c r="M84" s="38"/>
-      <c r="N84" s="39"/>
-      <c r="O84" s="39"/>
-      <c r="P84" s="39"/>
-      <c r="Q84" s="39"/>
-      <c r="R84" s="39"/>
-      <c r="S84" s="38"/>
-      <c r="T84" s="38"/>
-      <c r="U84" s="42"/>
+      <c r="J84" s="37"/>
+      <c r="K84" s="37"/>
+      <c r="L84" s="37"/>
+      <c r="M84" s="37"/>
+      <c r="N84" s="38"/>
+      <c r="O84" s="38"/>
+      <c r="P84" s="38"/>
+      <c r="Q84" s="38"/>
+      <c r="R84" s="38"/>
+      <c r="S84" s="37"/>
+      <c r="T84" s="37"/>
+      <c r="U84" s="41"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="B85" s="37" t="s">
+      <c r="B85" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="C85" s="37"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="37"/>
-      <c r="G85" s="37"/>
-      <c r="H85" s="38"/>
-      <c r="I85" s="38"/>
-      <c r="J85" s="38"/>
-      <c r="K85" s="38"/>
-      <c r="L85" s="38"/>
-      <c r="M85" s="38" t="s">
+      <c r="C85" s="36"/>
+      <c r="D85" s="36"/>
+      <c r="E85" s="36"/>
+      <c r="F85" s="36"/>
+      <c r="G85" s="36"/>
+      <c r="H85" s="37"/>
+      <c r="I85" s="37"/>
+      <c r="J85" s="37"/>
+      <c r="K85" s="37"/>
+      <c r="L85" s="37"/>
+      <c r="M85" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="N85" s="39"/>
-      <c r="O85" s="39"/>
-      <c r="P85" s="39"/>
-      <c r="Q85" s="39"/>
-      <c r="R85" s="39"/>
-      <c r="S85" s="38"/>
-      <c r="T85" s="38"/>
-      <c r="U85" s="43"/>
+      <c r="N85" s="38"/>
+      <c r="O85" s="38"/>
+      <c r="P85" s="38"/>
+      <c r="Q85" s="38"/>
+      <c r="R85" s="38"/>
+      <c r="S85" s="37"/>
+      <c r="T85" s="37"/>
+      <c r="U85" s="42"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="B86" s="44" t="s">
+      <c r="B86" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="C86" s="44"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="44"/>
-      <c r="F86" s="44"/>
-      <c r="G86" s="44"/>
-      <c r="H86" s="38"/>
-      <c r="I86" s="38"/>
-      <c r="J86" s="38"/>
-      <c r="K86" s="38"/>
-      <c r="L86" s="38"/>
-      <c r="M86" s="38"/>
-      <c r="N86" s="40"/>
-      <c r="O86" s="40"/>
-      <c r="P86" s="40"/>
-      <c r="Q86" s="40"/>
-      <c r="R86" s="40"/>
-      <c r="S86" s="38"/>
-      <c r="T86" s="38"/>
-      <c r="U86" s="42"/>
+      <c r="C86" s="43"/>
+      <c r="D86" s="43"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="43"/>
+      <c r="G86" s="43"/>
+      <c r="H86" s="37"/>
+      <c r="I86" s="37"/>
+      <c r="J86" s="37"/>
+      <c r="K86" s="37"/>
+      <c r="L86" s="37"/>
+      <c r="M86" s="37"/>
+      <c r="N86" s="39"/>
+      <c r="O86" s="39"/>
+      <c r="P86" s="39"/>
+      <c r="Q86" s="39"/>
+      <c r="R86" s="39"/>
+      <c r="S86" s="37"/>
+      <c r="T86" s="37"/>
+      <c r="U86" s="41"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="B87" s="37" t="s">
+      <c r="B87" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="C87" s="37"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="37"/>
-      <c r="G87" s="37"/>
-      <c r="H87" s="38"/>
-      <c r="I87" s="38"/>
-      <c r="J87" s="38"/>
-      <c r="K87" s="38"/>
-      <c r="L87" s="38"/>
-      <c r="M87" s="38"/>
-      <c r="N87" s="39"/>
-      <c r="O87" s="39"/>
-      <c r="P87" s="39"/>
-      <c r="Q87" s="39"/>
-      <c r="R87" s="39" t="s">
+      <c r="C87" s="36"/>
+      <c r="D87" s="36"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="36"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="37"/>
+      <c r="I87" s="37"/>
+      <c r="J87" s="37"/>
+      <c r="K87" s="37"/>
+      <c r="L87" s="37"/>
+      <c r="M87" s="37"/>
+      <c r="N87" s="38"/>
+      <c r="O87" s="38"/>
+      <c r="P87" s="38"/>
+      <c r="Q87" s="38"/>
+      <c r="R87" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="S87" s="38"/>
-      <c r="T87" s="38"/>
-      <c r="U87" s="43"/>
+      <c r="S87" s="37"/>
+      <c r="T87" s="37"/>
+      <c r="U87" s="42"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="20" t="n">
         <v>6</v>
       </c>
-      <c r="B88" s="37" t="s">
+      <c r="B88" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="C88" s="37"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="37"/>
-      <c r="G88" s="37"/>
-      <c r="H88" s="38"/>
-      <c r="I88" s="38"/>
-      <c r="J88" s="38"/>
-      <c r="K88" s="38"/>
-      <c r="L88" s="38"/>
-      <c r="M88" s="38"/>
-      <c r="N88" s="38"/>
-      <c r="O88" s="38"/>
-      <c r="P88" s="38"/>
-      <c r="Q88" s="38"/>
-      <c r="R88" s="38"/>
-      <c r="S88" s="38" t="s">
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="36"/>
+      <c r="F88" s="36"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="37"/>
+      <c r="I88" s="37"/>
+      <c r="J88" s="37"/>
+      <c r="K88" s="37"/>
+      <c r="L88" s="37"/>
+      <c r="M88" s="37"/>
+      <c r="N88" s="37"/>
+      <c r="O88" s="37"/>
+      <c r="P88" s="37"/>
+      <c r="Q88" s="37"/>
+      <c r="R88" s="37"/>
+      <c r="S88" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="T88" s="38"/>
-      <c r="U88" s="42"/>
+      <c r="T88" s="37"/>
+      <c r="U88" s="41"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4415,1427 +4062,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
-  </sheetPr>
-  <dimension ref="A1:AD34"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.14"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="6" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="4.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="0" width="8.71"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="2" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45"/>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="45"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48" t="n">
-        <f aca="false">Basplan!D2</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="48"/>
-      <c r="AC2" s="48"/>
-      <c r="AD2" s="48"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51" t="n">
-        <f aca="false">Basplan!D3</f>
-        <v>2</v>
-      </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="52"/>
-      <c r="AC3" s="52"/>
-      <c r="AD3" s="52"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="53" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55" t="n">
-        <f aca="false">Basplan!D4</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56"/>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="56"/>
-      <c r="Z4" s="56"/>
-      <c r="AA4" s="56"/>
-      <c r="AB4" s="56"/>
-      <c r="AC4" s="56"/>
-      <c r="AD4" s="56"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59" t="n">
-        <f aca="false">Basplan!D5</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="60"/>
-      <c r="U5" s="60"/>
-      <c r="V5" s="60"/>
-      <c r="W5" s="60"/>
-      <c r="X5" s="60"/>
-      <c r="Y5" s="60"/>
-      <c r="Z5" s="60"/>
-      <c r="AA5" s="60"/>
-      <c r="AB5" s="60"/>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="60"/>
-    </row>
-    <row r="6" s="17" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="H6" s="62"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
-      <c r="T6" s="62"/>
-      <c r="U6" s="62"/>
-      <c r="V6" s="62"/>
-      <c r="W6" s="62"/>
-      <c r="X6" s="62"/>
-      <c r="Y6" s="62"/>
-      <c r="Z6" s="62"/>
-      <c r="AA6" s="62"/>
-      <c r="AB6" s="62"/>
-      <c r="AC6" s="62"/>
-      <c r="AD6" s="62"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="63"/>
-      <c r="B7" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="18" t="n">
-        <f aca="false">Basplan!H7</f>
-        <v>40</v>
-      </c>
-      <c r="H7" s="65" t="n">
-        <f aca="false">Basplan!I7</f>
-        <v>41</v>
-      </c>
-      <c r="I7" s="65" t="n">
-        <f aca="false">Basplan!J7</f>
-        <v>42</v>
-      </c>
-      <c r="J7" s="65" t="n">
-        <f aca="false">Basplan!K7</f>
-        <v>43</v>
-      </c>
-      <c r="K7" s="65" t="n">
-        <f aca="false">Basplan!L7</f>
-        <v>44</v>
-      </c>
-      <c r="L7" s="65" t="n">
-        <f aca="false">Basplan!M7</f>
-        <v>45</v>
-      </c>
-      <c r="M7" s="65" t="n">
-        <f aca="false">Basplan!N7</f>
-        <v>46</v>
-      </c>
-      <c r="N7" s="65" t="n">
-        <f aca="false">Basplan!O7</f>
-        <v>47</v>
-      </c>
-      <c r="O7" s="65" t="n">
-        <f aca="false">Basplan!P7</f>
-        <v>48</v>
-      </c>
-      <c r="P7" s="65" t="n">
-        <f aca="false">Basplan!Q7</f>
-        <v>49</v>
-      </c>
-      <c r="Q7" s="65" t="n">
-        <f aca="false">Basplan!R7</f>
-        <v>50</v>
-      </c>
-      <c r="R7" s="65" t="n">
-        <f aca="false">Basplan!S7</f>
-        <v>51</v>
-      </c>
-      <c r="S7" s="65" t="n">
-        <f aca="false">Basplan!T7</f>
-        <v>52</v>
-      </c>
-      <c r="T7" s="65" t="n">
-        <f aca="false">Basplan!U7</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="65" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="V7" s="65" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="W7" s="65" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="X7" s="65" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Y7" s="65" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Z7" s="65" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AA7" s="65" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AB7" s="65" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AC7" s="65" t="e">
-        <f aca="false">#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="AD7" s="66" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="67"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
-      <c r="N8" s="70"/>
-      <c r="O8" s="70"/>
-      <c r="P8" s="70"/>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
-      <c r="Y8" s="70"/>
-      <c r="Z8" s="70"/>
-      <c r="AA8" s="70"/>
-      <c r="AB8" s="70"/>
-      <c r="AC8" s="71"/>
-      <c r="AD8" s="72" t="n">
-        <f aca="false">SUM(G8:AC8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="67"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75"/>
-      <c r="S9" s="75"/>
-      <c r="T9" s="75"/>
-      <c r="U9" s="75"/>
-      <c r="V9" s="75"/>
-      <c r="W9" s="75"/>
-      <c r="X9" s="75"/>
-      <c r="Y9" s="75"/>
-      <c r="Z9" s="75"/>
-      <c r="AA9" s="75"/>
-      <c r="AB9" s="75"/>
-      <c r="AC9" s="76"/>
-      <c r="AD9" s="77" t="n">
-        <f aca="false">SUM(G9:AC9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="67"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="75"/>
-      <c r="P10" s="75"/>
-      <c r="Q10" s="75"/>
-      <c r="R10" s="75"/>
-      <c r="S10" s="75"/>
-      <c r="T10" s="75"/>
-      <c r="U10" s="75"/>
-      <c r="V10" s="75"/>
-      <c r="W10" s="75"/>
-      <c r="X10" s="75"/>
-      <c r="Y10" s="75"/>
-      <c r="Z10" s="75"/>
-      <c r="AA10" s="75"/>
-      <c r="AB10" s="75"/>
-      <c r="AC10" s="76"/>
-      <c r="AD10" s="77" t="n">
-        <f aca="false">SUM(G10:AC10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="67"/>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="75"/>
-      <c r="P11" s="75"/>
-      <c r="Q11" s="75"/>
-      <c r="R11" s="75"/>
-      <c r="S11" s="75"/>
-      <c r="T11" s="75"/>
-      <c r="U11" s="75"/>
-      <c r="V11" s="75"/>
-      <c r="W11" s="75"/>
-      <c r="X11" s="75"/>
-      <c r="Y11" s="75"/>
-      <c r="Z11" s="75"/>
-      <c r="AA11" s="75"/>
-      <c r="AB11" s="75"/>
-      <c r="AC11" s="76"/>
-      <c r="AD11" s="77" t="n">
-        <f aca="false">SUM(G11:AC11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="67"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="75"/>
-      <c r="J12" s="75"/>
-      <c r="K12" s="75"/>
-      <c r="L12" s="75"/>
-      <c r="M12" s="75"/>
-      <c r="N12" s="75"/>
-      <c r="O12" s="75"/>
-      <c r="P12" s="75"/>
-      <c r="Q12" s="75"/>
-      <c r="R12" s="75"/>
-      <c r="S12" s="75"/>
-      <c r="T12" s="75"/>
-      <c r="U12" s="75"/>
-      <c r="V12" s="75"/>
-      <c r="W12" s="75"/>
-      <c r="X12" s="75"/>
-      <c r="Y12" s="75"/>
-      <c r="Z12" s="75"/>
-      <c r="AA12" s="75"/>
-      <c r="AB12" s="75"/>
-      <c r="AC12" s="76"/>
-      <c r="AD12" s="77" t="n">
-        <f aca="false">SUM(G12:AC12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="67"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="75"/>
-      <c r="M13" s="75"/>
-      <c r="N13" s="75"/>
-      <c r="O13" s="75"/>
-      <c r="P13" s="75"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="75"/>
-      <c r="S13" s="75"/>
-      <c r="T13" s="75"/>
-      <c r="U13" s="75"/>
-      <c r="V13" s="75"/>
-      <c r="W13" s="75"/>
-      <c r="X13" s="75"/>
-      <c r="Y13" s="75"/>
-      <c r="Z13" s="75"/>
-      <c r="AA13" s="75"/>
-      <c r="AB13" s="75"/>
-      <c r="AC13" s="76"/>
-      <c r="AD13" s="77" t="n">
-        <f aca="false">SUM(G13:AC13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="67"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="75"/>
-      <c r="N14" s="75"/>
-      <c r="O14" s="75"/>
-      <c r="P14" s="75"/>
-      <c r="Q14" s="75"/>
-      <c r="R14" s="75"/>
-      <c r="S14" s="75"/>
-      <c r="T14" s="75"/>
-      <c r="U14" s="75"/>
-      <c r="V14" s="75"/>
-      <c r="W14" s="75"/>
-      <c r="X14" s="75"/>
-      <c r="Y14" s="75"/>
-      <c r="Z14" s="75"/>
-      <c r="AA14" s="75"/>
-      <c r="AB14" s="75"/>
-      <c r="AC14" s="76"/>
-      <c r="AD14" s="77" t="n">
-        <f aca="false">SUM(G14:AC14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="67"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="73"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="75"/>
-      <c r="L15" s="75"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="75"/>
-      <c r="P15" s="75"/>
-      <c r="Q15" s="75"/>
-      <c r="R15" s="75"/>
-      <c r="S15" s="75"/>
-      <c r="T15" s="75"/>
-      <c r="U15" s="75"/>
-      <c r="V15" s="75"/>
-      <c r="W15" s="75"/>
-      <c r="X15" s="75"/>
-      <c r="Y15" s="75"/>
-      <c r="Z15" s="75"/>
-      <c r="AA15" s="75"/>
-      <c r="AB15" s="75"/>
-      <c r="AC15" s="76"/>
-      <c r="AD15" s="77" t="n">
-        <f aca="false">SUM(G15:AC15)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="67"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="75"/>
-      <c r="L16" s="75"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75"/>
-      <c r="O16" s="75"/>
-      <c r="P16" s="75"/>
-      <c r="Q16" s="75"/>
-      <c r="R16" s="75"/>
-      <c r="S16" s="75"/>
-      <c r="T16" s="75"/>
-      <c r="U16" s="75"/>
-      <c r="V16" s="75"/>
-      <c r="W16" s="75"/>
-      <c r="X16" s="75"/>
-      <c r="Y16" s="75"/>
-      <c r="Z16" s="75"/>
-      <c r="AA16" s="75"/>
-      <c r="AB16" s="75"/>
-      <c r="AC16" s="76"/>
-      <c r="AD16" s="77" t="n">
-        <f aca="false">SUM(G16:AC16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="67"/>
-      <c r="B17" s="73"/>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="75"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="75"/>
-      <c r="P17" s="75"/>
-      <c r="Q17" s="75"/>
-      <c r="R17" s="75"/>
-      <c r="S17" s="75"/>
-      <c r="T17" s="75"/>
-      <c r="U17" s="75"/>
-      <c r="V17" s="75"/>
-      <c r="W17" s="75"/>
-      <c r="X17" s="75"/>
-      <c r="Y17" s="75"/>
-      <c r="Z17" s="75"/>
-      <c r="AA17" s="75"/>
-      <c r="AB17" s="75"/>
-      <c r="AC17" s="76"/>
-      <c r="AD17" s="77" t="n">
-        <f aca="false">SUM(G17:AC17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="67"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
-      <c r="L18" s="75"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
-      <c r="Q18" s="75"/>
-      <c r="R18" s="75"/>
-      <c r="S18" s="75"/>
-      <c r="T18" s="75"/>
-      <c r="U18" s="75"/>
-      <c r="V18" s="75"/>
-      <c r="W18" s="75"/>
-      <c r="X18" s="75"/>
-      <c r="Y18" s="75"/>
-      <c r="Z18" s="75"/>
-      <c r="AA18" s="75"/>
-      <c r="AB18" s="75"/>
-      <c r="AC18" s="76"/>
-      <c r="AD18" s="77" t="n">
-        <f aca="false">SUM(G18:AC18)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="67"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="75"/>
-      <c r="Q19" s="75"/>
-      <c r="R19" s="75"/>
-      <c r="S19" s="75"/>
-      <c r="T19" s="75"/>
-      <c r="U19" s="75"/>
-      <c r="V19" s="75"/>
-      <c r="W19" s="75"/>
-      <c r="X19" s="75"/>
-      <c r="Y19" s="75"/>
-      <c r="Z19" s="75"/>
-      <c r="AA19" s="75"/>
-      <c r="AB19" s="75"/>
-      <c r="AC19" s="76"/>
-      <c r="AD19" s="77" t="n">
-        <f aca="false">SUM(G19:AC19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="67"/>
-      <c r="B20" s="73"/>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="75"/>
-      <c r="I20" s="75"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="75"/>
-      <c r="L20" s="75"/>
-      <c r="M20" s="75"/>
-      <c r="N20" s="75"/>
-      <c r="O20" s="75"/>
-      <c r="P20" s="75"/>
-      <c r="Q20" s="75"/>
-      <c r="R20" s="75"/>
-      <c r="S20" s="75"/>
-      <c r="T20" s="75"/>
-      <c r="U20" s="75"/>
-      <c r="V20" s="75"/>
-      <c r="W20" s="75"/>
-      <c r="X20" s="75"/>
-      <c r="Y20" s="75"/>
-      <c r="Z20" s="75"/>
-      <c r="AA20" s="75"/>
-      <c r="AB20" s="75"/>
-      <c r="AC20" s="76"/>
-      <c r="AD20" s="77" t="n">
-        <f aca="false">SUM(G20:AC20)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="67"/>
-      <c r="B21" s="73"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="75"/>
-      <c r="N21" s="75"/>
-      <c r="O21" s="75"/>
-      <c r="P21" s="75"/>
-      <c r="Q21" s="75"/>
-      <c r="R21" s="75"/>
-      <c r="S21" s="75"/>
-      <c r="T21" s="75"/>
-      <c r="U21" s="75"/>
-      <c r="V21" s="75"/>
-      <c r="W21" s="75"/>
-      <c r="X21" s="75"/>
-      <c r="Y21" s="75"/>
-      <c r="Z21" s="75"/>
-      <c r="AA21" s="75"/>
-      <c r="AB21" s="75"/>
-      <c r="AC21" s="76"/>
-      <c r="AD21" s="77" t="n">
-        <f aca="false">SUM(G21:AC21)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="67"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="75"/>
-      <c r="I22" s="75"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="75"/>
-      <c r="M22" s="75"/>
-      <c r="N22" s="75"/>
-      <c r="O22" s="75"/>
-      <c r="P22" s="75"/>
-      <c r="Q22" s="75"/>
-      <c r="R22" s="75"/>
-      <c r="S22" s="75"/>
-      <c r="T22" s="75"/>
-      <c r="U22" s="75"/>
-      <c r="V22" s="75"/>
-      <c r="W22" s="75"/>
-      <c r="X22" s="75"/>
-      <c r="Y22" s="75"/>
-      <c r="Z22" s="75"/>
-      <c r="AA22" s="75"/>
-      <c r="AB22" s="75"/>
-      <c r="AC22" s="76"/>
-      <c r="AD22" s="77" t="n">
-        <f aca="false">SUM(G22:AC22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="67"/>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="75"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="75"/>
-      <c r="L23" s="75"/>
-      <c r="M23" s="75"/>
-      <c r="N23" s="75"/>
-      <c r="O23" s="75"/>
-      <c r="P23" s="75"/>
-      <c r="Q23" s="75"/>
-      <c r="R23" s="75"/>
-      <c r="S23" s="75"/>
-      <c r="T23" s="75"/>
-      <c r="U23" s="75"/>
-      <c r="V23" s="75"/>
-      <c r="W23" s="75"/>
-      <c r="X23" s="75"/>
-      <c r="Y23" s="75"/>
-      <c r="Z23" s="75"/>
-      <c r="AA23" s="75"/>
-      <c r="AB23" s="75"/>
-      <c r="AC23" s="76"/>
-      <c r="AD23" s="77" t="n">
-        <f aca="false">SUM(G23:AC23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="67"/>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
-      <c r="N24" s="75"/>
-      <c r="O24" s="75"/>
-      <c r="P24" s="75"/>
-      <c r="Q24" s="75"/>
-      <c r="R24" s="75"/>
-      <c r="S24" s="75"/>
-      <c r="T24" s="75"/>
-      <c r="U24" s="75"/>
-      <c r="V24" s="75"/>
-      <c r="W24" s="75"/>
-      <c r="X24" s="75"/>
-      <c r="Y24" s="75"/>
-      <c r="Z24" s="75"/>
-      <c r="AA24" s="75"/>
-      <c r="AB24" s="75"/>
-      <c r="AC24" s="76"/>
-      <c r="AD24" s="77" t="n">
-        <f aca="false">SUM(G24:AC24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="67"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="75"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="75"/>
-      <c r="K25" s="75"/>
-      <c r="L25" s="75"/>
-      <c r="M25" s="75"/>
-      <c r="N25" s="75"/>
-      <c r="O25" s="75"/>
-      <c r="P25" s="75"/>
-      <c r="Q25" s="75"/>
-      <c r="R25" s="75"/>
-      <c r="S25" s="75"/>
-      <c r="T25" s="75"/>
-      <c r="U25" s="75"/>
-      <c r="V25" s="75"/>
-      <c r="W25" s="75"/>
-      <c r="X25" s="75"/>
-      <c r="Y25" s="75"/>
-      <c r="Z25" s="75"/>
-      <c r="AA25" s="75"/>
-      <c r="AB25" s="75"/>
-      <c r="AC25" s="76"/>
-      <c r="AD25" s="77" t="n">
-        <f aca="false">SUM(G25:AC25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="67"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="75"/>
-      <c r="K26" s="75"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="75"/>
-      <c r="N26" s="75"/>
-      <c r="O26" s="75"/>
-      <c r="P26" s="75"/>
-      <c r="Q26" s="75"/>
-      <c r="R26" s="75"/>
-      <c r="S26" s="75"/>
-      <c r="T26" s="75"/>
-      <c r="U26" s="75"/>
-      <c r="V26" s="75"/>
-      <c r="W26" s="75"/>
-      <c r="X26" s="75"/>
-      <c r="Y26" s="75"/>
-      <c r="Z26" s="75"/>
-      <c r="AA26" s="75"/>
-      <c r="AB26" s="75"/>
-      <c r="AC26" s="76"/>
-      <c r="AD26" s="77" t="n">
-        <f aca="false">SUM(G26:AC26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="67"/>
-      <c r="B27" s="73"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
-      <c r="M27" s="75"/>
-      <c r="N27" s="75"/>
-      <c r="O27" s="75"/>
-      <c r="P27" s="75"/>
-      <c r="Q27" s="75"/>
-      <c r="R27" s="75"/>
-      <c r="S27" s="75"/>
-      <c r="T27" s="75"/>
-      <c r="U27" s="75"/>
-      <c r="V27" s="75"/>
-      <c r="W27" s="75"/>
-      <c r="X27" s="75"/>
-      <c r="Y27" s="75"/>
-      <c r="Z27" s="75"/>
-      <c r="AA27" s="75"/>
-      <c r="AB27" s="75"/>
-      <c r="AC27" s="76"/>
-      <c r="AD27" s="77" t="n">
-        <f aca="false">SUM(G27:AC27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="78"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="75"/>
-      <c r="J28" s="75"/>
-      <c r="K28" s="75"/>
-      <c r="L28" s="75"/>
-      <c r="M28" s="75"/>
-      <c r="N28" s="75"/>
-      <c r="O28" s="75"/>
-      <c r="P28" s="75"/>
-      <c r="Q28" s="75"/>
-      <c r="R28" s="75"/>
-      <c r="S28" s="75"/>
-      <c r="T28" s="75"/>
-      <c r="U28" s="75"/>
-      <c r="V28" s="75"/>
-      <c r="W28" s="75"/>
-      <c r="X28" s="75"/>
-      <c r="Y28" s="75"/>
-      <c r="Z28" s="75"/>
-      <c r="AA28" s="75"/>
-      <c r="AB28" s="75"/>
-      <c r="AC28" s="76"/>
-      <c r="AD28" s="77" t="n">
-        <f aca="false">SUM(G28:AC28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="78"/>
-      <c r="B29" s="73"/>
-      <c r="C29" s="73"/>
-      <c r="D29" s="73"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="75"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="75"/>
-      <c r="M29" s="75"/>
-      <c r="N29" s="75"/>
-      <c r="O29" s="75"/>
-      <c r="P29" s="75"/>
-      <c r="Q29" s="75"/>
-      <c r="R29" s="75"/>
-      <c r="S29" s="75"/>
-      <c r="T29" s="75"/>
-      <c r="U29" s="75"/>
-      <c r="V29" s="75"/>
-      <c r="W29" s="75"/>
-      <c r="X29" s="75"/>
-      <c r="Y29" s="75"/>
-      <c r="Z29" s="75"/>
-      <c r="AA29" s="75"/>
-      <c r="AB29" s="75"/>
-      <c r="AC29" s="76"/>
-      <c r="AD29" s="77" t="n">
-        <f aca="false">SUM(G29:AC29)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="67"/>
-      <c r="B30" s="73"/>
-      <c r="C30" s="73"/>
-      <c r="D30" s="73"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="75"/>
-      <c r="L30" s="75"/>
-      <c r="M30" s="75"/>
-      <c r="N30" s="75"/>
-      <c r="O30" s="75"/>
-      <c r="P30" s="75"/>
-      <c r="Q30" s="75"/>
-      <c r="R30" s="75"/>
-      <c r="S30" s="75"/>
-      <c r="T30" s="75"/>
-      <c r="U30" s="75"/>
-      <c r="V30" s="75"/>
-      <c r="W30" s="75"/>
-      <c r="X30" s="75"/>
-      <c r="Y30" s="75"/>
-      <c r="Z30" s="75"/>
-      <c r="AA30" s="75"/>
-      <c r="AB30" s="75"/>
-      <c r="AC30" s="76"/>
-      <c r="AD30" s="77" t="n">
-        <f aca="false">SUM(G30:AC30)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="67"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="75"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="75"/>
-      <c r="L31" s="75"/>
-      <c r="M31" s="75"/>
-      <c r="N31" s="75"/>
-      <c r="O31" s="75"/>
-      <c r="P31" s="75"/>
-      <c r="Q31" s="75"/>
-      <c r="R31" s="75"/>
-      <c r="S31" s="75"/>
-      <c r="T31" s="75"/>
-      <c r="U31" s="75"/>
-      <c r="V31" s="75"/>
-      <c r="W31" s="75"/>
-      <c r="X31" s="75"/>
-      <c r="Y31" s="75"/>
-      <c r="Z31" s="75"/>
-      <c r="AA31" s="75"/>
-      <c r="AB31" s="75"/>
-      <c r="AC31" s="76"/>
-      <c r="AD31" s="77" t="n">
-        <f aca="false">SUM(G31:AC31)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="67"/>
-      <c r="B32" s="73"/>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
-      <c r="E32" s="73"/>
-      <c r="F32" s="73"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="75"/>
-      <c r="L32" s="75"/>
-      <c r="M32" s="75"/>
-      <c r="N32" s="75"/>
-      <c r="O32" s="75"/>
-      <c r="P32" s="75"/>
-      <c r="Q32" s="75"/>
-      <c r="R32" s="75"/>
-      <c r="S32" s="75"/>
-      <c r="T32" s="75"/>
-      <c r="U32" s="75"/>
-      <c r="V32" s="75"/>
-      <c r="W32" s="75"/>
-      <c r="X32" s="75"/>
-      <c r="Y32" s="75"/>
-      <c r="Z32" s="75"/>
-      <c r="AA32" s="75"/>
-      <c r="AB32" s="75"/>
-      <c r="AC32" s="76"/>
-      <c r="AD32" s="77" t="n">
-        <f aca="false">SUM(G32:AC32)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="67"/>
-      <c r="B33" s="79"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="80"/>
-      <c r="H33" s="81"/>
-      <c r="I33" s="81"/>
-      <c r="J33" s="81"/>
-      <c r="K33" s="81"/>
-      <c r="L33" s="81"/>
-      <c r="M33" s="81"/>
-      <c r="N33" s="81"/>
-      <c r="O33" s="81"/>
-      <c r="P33" s="81"/>
-      <c r="Q33" s="81"/>
-      <c r="R33" s="81"/>
-      <c r="S33" s="81"/>
-      <c r="T33" s="81"/>
-      <c r="U33" s="81"/>
-      <c r="V33" s="81"/>
-      <c r="W33" s="81"/>
-      <c r="X33" s="81"/>
-      <c r="Y33" s="81"/>
-      <c r="Z33" s="81"/>
-      <c r="AA33" s="81"/>
-      <c r="AB33" s="81"/>
-      <c r="AC33" s="82"/>
-      <c r="AD33" s="77" t="n">
-        <f aca="false">SUM(G33:AC33)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="18"/>
-      <c r="B34" s="83" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" s="83"/>
-      <c r="D34" s="83"/>
-      <c r="E34" s="83"/>
-      <c r="F34" s="83"/>
-      <c r="G34" s="84" t="n">
-        <f aca="false">SUM(G8:G33)</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="84" t="n">
-        <f aca="false">SUM(H8:H33)</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="84" t="n">
-        <f aca="false">SUM(I8:I33)</f>
-        <v>0</v>
-      </c>
-      <c r="J34" s="84" t="n">
-        <f aca="false">SUM(J8:J33)</f>
-        <v>0</v>
-      </c>
-      <c r="K34" s="84" t="n">
-        <f aca="false">SUM(K8:K33)</f>
-        <v>0</v>
-      </c>
-      <c r="L34" s="84" t="n">
-        <f aca="false">SUM(L8:L33)</f>
-        <v>0</v>
-      </c>
-      <c r="M34" s="84" t="n">
-        <f aca="false">SUM(M8:M33)</f>
-        <v>0</v>
-      </c>
-      <c r="N34" s="84" t="n">
-        <f aca="false">SUM(N8:N33)</f>
-        <v>0</v>
-      </c>
-      <c r="O34" s="84" t="n">
-        <f aca="false">SUM(O8:O33)</f>
-        <v>0</v>
-      </c>
-      <c r="P34" s="84" t="n">
-        <f aca="false">SUM(P8:P33)</f>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="84" t="n">
-        <f aca="false">SUM(Q8:Q33)</f>
-        <v>0</v>
-      </c>
-      <c r="R34" s="84" t="n">
-        <f aca="false">SUM(R8:R33)</f>
-        <v>0</v>
-      </c>
-      <c r="S34" s="84" t="n">
-        <f aca="false">SUM(S8:S33)</f>
-        <v>0</v>
-      </c>
-      <c r="T34" s="84" t="n">
-        <f aca="false">SUM(T8:T33)</f>
-        <v>0</v>
-      </c>
-      <c r="U34" s="84" t="n">
-        <f aca="false">SUM(U8:U33)</f>
-        <v>0</v>
-      </c>
-      <c r="V34" s="84" t="n">
-        <f aca="false">SUM(V8:V33)</f>
-        <v>0</v>
-      </c>
-      <c r="W34" s="84" t="n">
-        <f aca="false">SUM(W8:W33)</f>
-        <v>0</v>
-      </c>
-      <c r="X34" s="84" t="n">
-        <f aca="false">SUM(X8:X33)</f>
-        <v>0</v>
-      </c>
-      <c r="Y34" s="84" t="n">
-        <f aca="false">SUM(Y8:Y33)</f>
-        <v>0</v>
-      </c>
-      <c r="Z34" s="84" t="n">
-        <f aca="false">SUM(Z8:Z33)</f>
-        <v>0</v>
-      </c>
-      <c r="AA34" s="84" t="n">
-        <f aca="false">SUM(AA8:AA33)</f>
-        <v>0</v>
-      </c>
-      <c r="AB34" s="84" t="n">
-        <f aca="false">SUM(AB8:AB33)</f>
-        <v>0</v>
-      </c>
-      <c r="AC34" s="84" t="n">
-        <f aca="false">SUM(AC8:AC33)</f>
-        <v>0</v>
-      </c>
-      <c r="AD34" s="85" t="n">
-        <f aca="false">SUM(AD8:AD33)</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:AD2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:AD3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:AD4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:AD5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="G6:AD6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.709722222222222" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>